<commit_message>
remove columns and rows
</commit_message>
<xml_diff>
--- a/src/data/Acompanhamento Orçamento OPEX - Agosto2024 - Copia.xlsx
+++ b/src/data/Acompanhamento Orçamento OPEX - Agosto2024 - Copia.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anderson\Desktop\OPEX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anderson.bones\Desktop\Projetos\Python\opex-fs\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFAA4B0F-91F5-4941-B591-237522F692C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C47B194-87FB-4210-8DC2-10A9FD645D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="552" windowWidth="23016" windowHeight="11688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meses" sheetId="1" r:id="rId1"/>
@@ -22,21 +22,34 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
-    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="9" r:id="rId4"/>
+    <pivotCache cacheId="10" r:id="rId5"/>
   </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -1294,6 +1307,28 @@
     <xf numFmtId="166" fontId="0" fillId="9" borderId="9" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1363,28 +1398,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Moeda" xfId="2" builtinId="4"/>
@@ -1393,6 +1406,9 @@
     <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="32">
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
     <dxf>
       <border>
         <left style="medium">
@@ -1712,9 +1728,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -2391,28 +2404,28 @@
             <c:strLit>
               <c:ptCount val="8"/>
               <c:pt idx="0">
-                <c:v>100%</c:v>
+                <c:v>1</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>200%</c:v>
+                <c:v>2</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v>300%</c:v>
+                <c:v>3</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>400%</c:v>
+                <c:v>4</c:v>
               </c:pt>
               <c:pt idx="4">
-                <c:v>500%</c:v>
+                <c:v>5</c:v>
               </c:pt>
               <c:pt idx="5">
-                <c:v>600%</c:v>
+                <c:v>6</c:v>
               </c:pt>
               <c:pt idx="6">
-                <c:v>700%</c:v>
+                <c:v>7</c:v>
               </c:pt>
               <c:pt idx="7">
-                <c:v>800%</c:v>
+                <c:v>8</c:v>
               </c:pt>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -5779,7 +5792,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CABA5277-C369-4823-82A1-268B72B3CD5C}" name="Tabela dinâmica21" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="26" rowHeaderCaption="Despesa">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CABA5277-C369-4823-82A1-268B72B3CD5C}" name="Tabela dinâmica21" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="26" rowHeaderCaption="Despesa">
   <location ref="I6:L15" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -5852,23 +5865,32 @@
     <dataField name="Soma de Δ Fct x Bdg" fld="4" baseField="0" baseItem="0" numFmtId="167"/>
   </dataFields>
   <formats count="31">
-    <format dxfId="30">
+    <format dxfId="31">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="29">
+    <format dxfId="30">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="29">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
             <x v="2"/>
           </reference>
           <reference field="0" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="28">
+      <pivotArea field="0" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
         </references>
       </pivotArea>
     </format>
@@ -5909,7 +5931,7 @@
       </pivotArea>
     </format>
     <format dxfId="23">
-      <pivotArea field="0" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="2"/>
@@ -5927,18 +5949,9 @@
       </pivotArea>
     </format>
     <format dxfId="21">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
     <format dxfId="20">
-      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="19">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -5949,29 +5962,29 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="19">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="17">
+    <format dxfId="18">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="16">
+    <format dxfId="17">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="15">
+    <format dxfId="16">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="14">
+    <format dxfId="15">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="12">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -5982,26 +5995,26 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="12">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="10">
+    <format dxfId="11">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="9">
+    <format dxfId="10">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="8">
+    <format dxfId="9">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -6012,26 +6025,26 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="6">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="5">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="3">
+    <format dxfId="4">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="0">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -6239,17 +6252,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1">
         <x14:conditionalFormats count="2">
-          <x14:conditionalFormat priority="5" id="{57A22362-E8D4-43C1-8382-FF9EC3A2FC8B}">
-            <x14:pivotAreas count="1">
-              <pivotArea type="data" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-                <references count="1">
-                  <reference field="4294967294" count="1" selected="0">
-                    <x v="2"/>
-                  </reference>
-                </references>
-              </pivotArea>
-            </x14:pivotAreas>
-          </x14:conditionalFormat>
           <x14:conditionalFormat priority="6" id="{2F1A8382-0BB3-4B69-85C0-D1EEF9D80BA3}">
             <x14:pivotAreas count="1">
               <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
@@ -6271,6 +6273,17 @@
               </pivotArea>
             </x14:pivotAreas>
           </x14:conditionalFormat>
+          <x14:conditionalFormat priority="5" id="{57A22362-E8D4-43C1-8382-FF9EC3A2FC8B}">
+            <x14:pivotAreas count="1">
+              <pivotArea type="data" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+                <references count="1">
+                  <reference field="4294967294" count="1" selected="0">
+                    <x v="2"/>
+                  </reference>
+                </references>
+              </pivotArea>
+            </x14:pivotAreas>
+          </x14:conditionalFormat>
         </x14:conditionalFormats>
       </x14:pivotTableDefinition>
     </ext>
@@ -6282,7 +6295,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BB6324FA-1E30-400D-99B4-D79F50C7A0F6}" name="Tabela dinâmica1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BB6324FA-1E30-400D-99B4-D79F50C7A0F6}" name="Tabela dinâmica1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F2:S28" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -6501,7 +6514,7 @@
     <dataField name="Soma de Previsão" fld="3" baseField="0" baseItem="0" numFmtId="43"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="31">
+    <format dxfId="0">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -6841,77 +6854,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:AJ70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T55" sqref="T55"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="49.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="9.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.69921875" style="1" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="49.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="9.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.3984375" style="1" customWidth="1"/>
     <col min="20" max="20" width="11" style="1" customWidth="1"/>
     <col min="21" max="21" width="41" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="20.75" style="1"/>
+    <col min="22" max="16384" width="20.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="B4" s="108" t="s">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="B4" s="116" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="104" t="s">
+      <c r="C4" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="104" t="s">
+      <c r="D4" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="104" t="s">
+      <c r="E4" s="112" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="104"/>
-      <c r="G4" s="104"/>
-      <c r="H4" s="104" t="s">
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="112" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="104"/>
-      <c r="J4" s="104"/>
-      <c r="K4" s="104"/>
-      <c r="L4" s="104"/>
-      <c r="M4" s="104"/>
-      <c r="N4" s="104"/>
-      <c r="O4" s="104"/>
-      <c r="P4" s="104"/>
-      <c r="Q4" s="104" t="s">
+      <c r="I4" s="112"/>
+      <c r="J4" s="112"/>
+      <c r="K4" s="112"/>
+      <c r="L4" s="112"/>
+      <c r="M4" s="112"/>
+      <c r="N4" s="112"/>
+      <c r="O4" s="112"/>
+      <c r="P4" s="112"/>
+      <c r="Q4" s="112" t="s">
         <v>79</v>
       </c>
-      <c r="R4" s="104" t="s">
+      <c r="R4" s="112" t="s">
         <v>69</v>
       </c>
-      <c r="S4" s="104" t="s">
+      <c r="S4" s="112" t="s">
         <v>66</v>
       </c>
-      <c r="T4" s="104" t="s">
+      <c r="T4" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="U4" s="106" t="s">
+      <c r="U4" s="114" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="B5" s="109"/>
-      <c r="C5" s="105"/>
-      <c r="D5" s="105"/>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="B5" s="117"/>
+      <c r="C5" s="113"/>
+      <c r="D5" s="113"/>
       <c r="E5" s="25">
         <v>45383</v>
       </c>
@@ -6948,13 +6961,13 @@
       <c r="P5" s="25">
         <v>45717</v>
       </c>
-      <c r="Q5" s="105"/>
-      <c r="R5" s="105"/>
-      <c r="S5" s="105"/>
-      <c r="T5" s="105"/>
-      <c r="U5" s="107"/>
-    </row>
-    <row r="6" spans="1:36" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q5" s="113"/>
+      <c r="R5" s="113"/>
+      <c r="S5" s="113"/>
+      <c r="T5" s="113"/>
+      <c r="U5" s="115"/>
+    </row>
+    <row r="6" spans="1:36" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -6968,7 +6981,7 @@
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>49</v>
       </c>
@@ -7047,12 +7060,12 @@
       <c r="U7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="V7" s="127">
+      <c r="V7" s="104">
         <f>Q7-R7</f>
         <v>99813.228342604591</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B8"/>
       <c r="C8"/>
       <c r="D8"/>
@@ -7073,12 +7086,12 @@
       <c r="S8"/>
       <c r="T8"/>
       <c r="U8"/>
-      <c r="V8" s="127">
+      <c r="V8" s="104">
         <f t="shared" ref="V8:V13" si="3">Q8-R8</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B9" s="13" t="s">
         <v>5</v>
       </c>
@@ -7144,7 +7157,7 @@
       <c r="U9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="V9" s="127">
+      <c r="V9" s="104">
         <f t="shared" si="3"/>
         <v>1467.1563306749886</v>
       </c>
@@ -7163,7 +7176,7 @@
       <c r="AI9" s="8"/>
       <c r="AJ9" s="8"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>40120101</v>
       </c>
@@ -7225,7 +7238,7 @@
       <c r="U10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="V10" s="127">
+      <c r="V10" s="104">
         <f t="shared" si="3"/>
         <v>7035.1196640083326</v>
       </c>
@@ -7244,7 +7257,7 @@
       <c r="AI10" s="8"/>
       <c r="AJ10" s="8"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>40120102</v>
       </c>
@@ -7312,7 +7325,7 @@
       <c r="U11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="V11" s="127">
+      <c r="V11" s="104">
         <f t="shared" si="3"/>
         <v>-8426.7766666666721</v>
       </c>
@@ -7331,7 +7344,7 @@
       <c r="AI11" s="8"/>
       <c r="AJ11" s="8"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>40120103</v>
       </c>
@@ -7395,7 +7408,7 @@
       <c r="U12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="V12" s="127">
+      <c r="V12" s="104">
         <f t="shared" si="3"/>
         <v>2858.813333333334</v>
       </c>
@@ -7414,7 +7427,7 @@
       <c r="AI12" s="8"/>
       <c r="AJ12" s="8"/>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B13" s="13" t="s">
         <v>9</v>
       </c>
@@ -7478,7 +7491,7 @@
       <c r="U13" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="V13" s="127">
+      <c r="V13" s="104">
         <f t="shared" si="3"/>
         <v>109741.81</v>
       </c>
@@ -7497,7 +7510,7 @@
       <c r="AI13" s="8"/>
       <c r="AJ13" s="8"/>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>40120201</v>
       </c>
@@ -7579,7 +7592,7 @@
       <c r="AI14" s="8"/>
       <c r="AJ14" s="8"/>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B15" s="14"/>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -7616,7 +7629,7 @@
       <c r="AI15" s="8"/>
       <c r="AJ15" s="8"/>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B16" s="13" t="s">
         <v>11</v>
       </c>
@@ -7698,7 +7711,7 @@
       <c r="AI16" s="8"/>
       <c r="AJ16" s="8"/>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>40120401</v>
       </c>
@@ -7782,7 +7795,7 @@
       <c r="AI17" s="8"/>
       <c r="AJ17" s="8"/>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>40120402</v>
       </c>
@@ -7866,7 +7879,7 @@
       <c r="AI18" s="8"/>
       <c r="AJ18" s="8"/>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>40120403</v>
       </c>
@@ -7950,7 +7963,7 @@
       <c r="AI19" s="8"/>
       <c r="AJ19" s="8"/>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>40120404</v>
       </c>
@@ -8034,7 +8047,7 @@
       <c r="AI20" s="8"/>
       <c r="AJ20" s="8"/>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B21" s="14"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
@@ -8071,7 +8084,7 @@
       <c r="AI21" s="8"/>
       <c r="AJ21" s="8"/>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B22" s="13" t="s">
         <v>16</v>
       </c>
@@ -8153,7 +8166,7 @@
       <c r="AI22" s="8"/>
       <c r="AJ22" s="8"/>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>40120501</v>
       </c>
@@ -8237,7 +8250,7 @@
       <c r="AI23" s="8"/>
       <c r="AJ23" s="8"/>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>40120503</v>
       </c>
@@ -8321,7 +8334,7 @@
       <c r="AI24" s="8"/>
       <c r="AJ24" s="8"/>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B25" s="13" t="s">
         <v>19</v>
       </c>
@@ -8403,7 +8416,7 @@
       <c r="AI25" s="8"/>
       <c r="AJ25" s="8"/>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>40120601</v>
       </c>
@@ -8477,7 +8490,7 @@
       <c r="AI26" s="8"/>
       <c r="AJ26" s="8"/>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>40120602</v>
       </c>
@@ -8561,7 +8574,7 @@
       <c r="AI27" s="8"/>
       <c r="AJ27" s="8"/>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>40120605</v>
       </c>
@@ -8633,7 +8646,7 @@
       <c r="AI28" s="8"/>
       <c r="AJ28" s="8"/>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>40120603</v>
       </c>
@@ -8695,7 +8708,7 @@
       <c r="AI29" s="8"/>
       <c r="AJ29" s="8"/>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>40120606</v>
       </c>
@@ -8773,7 +8786,7 @@
       <c r="AI30" s="8"/>
       <c r="AJ30" s="8"/>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>40120612</v>
       </c>
@@ -8857,7 +8870,7 @@
       <c r="AI31" s="8"/>
       <c r="AJ31" s="8"/>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>40120613</v>
       </c>
@@ -8933,7 +8946,7 @@
       <c r="AI32" s="8"/>
       <c r="AJ32" s="8"/>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>40120614</v>
       </c>
@@ -9013,7 +9026,7 @@
       <c r="AI33" s="8"/>
       <c r="AJ33" s="8"/>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B34" s="14"/>
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
@@ -9050,7 +9063,7 @@
       <c r="AI34" s="8"/>
       <c r="AJ34" s="8"/>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B35" s="13" t="s">
         <v>27</v>
       </c>
@@ -9132,7 +9145,7 @@
       <c r="AI35" s="8"/>
       <c r="AJ35" s="8"/>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>40120701</v>
       </c>
@@ -9214,7 +9227,7 @@
       <c r="AI36" s="8"/>
       <c r="AJ36" s="8"/>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>40120705</v>
       </c>
@@ -9296,7 +9309,7 @@
       <c r="AI37" s="8"/>
       <c r="AJ37" s="8"/>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>40120706</v>
       </c>
@@ -9374,7 +9387,7 @@
       <c r="AI38" s="8"/>
       <c r="AJ38" s="8"/>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>40120707</v>
       </c>
@@ -9450,7 +9463,7 @@
       <c r="AI39" s="8"/>
       <c r="AJ39" s="8"/>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B40" s="14"/>
       <c r="C40" s="17"/>
       <c r="D40" s="17"/>
@@ -9487,7 +9500,7 @@
       <c r="AI40" s="8"/>
       <c r="AJ40" s="8"/>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B41" s="13" t="s">
         <v>32</v>
       </c>
@@ -9561,7 +9574,7 @@
       <c r="AI41" s="8"/>
       <c r="AJ41" s="8"/>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>40120801</v>
       </c>
@@ -9635,7 +9648,7 @@
       <c r="AI42" s="8"/>
       <c r="AJ42" s="8"/>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>40120804</v>
       </c>
@@ -9711,7 +9724,7 @@
       <c r="AI43" s="8"/>
       <c r="AJ43" s="8"/>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B44" s="14"/>
       <c r="C44" s="17"/>
       <c r="D44" s="17"/>
@@ -9748,7 +9761,7 @@
       <c r="AI44" s="8"/>
       <c r="AJ44" s="8"/>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B45" s="13" t="s">
         <v>35</v>
       </c>
@@ -9822,7 +9835,7 @@
       <c r="AI45" s="8"/>
       <c r="AJ45" s="8"/>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>40120901</v>
       </c>
@@ -9898,7 +9911,7 @@
       <c r="AI46" s="8"/>
       <c r="AJ46" s="8"/>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B47" s="14"/>
       <c r="C47" s="17"/>
       <c r="D47" s="17"/>
@@ -9935,7 +9948,7 @@
       <c r="AI47" s="8"/>
       <c r="AJ47" s="8"/>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B48" s="13" t="s">
         <v>37</v>
       </c>
@@ -10017,7 +10030,7 @@
       <c r="AI48" s="8"/>
       <c r="AJ48" s="8"/>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>40121102</v>
       </c>
@@ -10099,7 +10112,7 @@
       <c r="AI49" s="8"/>
       <c r="AJ49" s="8"/>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>40121104</v>
       </c>
@@ -10173,7 +10186,7 @@
       <c r="AI50" s="8"/>
       <c r="AJ50" s="8"/>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>40121107</v>
       </c>
@@ -10249,7 +10262,7 @@
       <c r="AI51" s="8"/>
       <c r="AJ51" s="8"/>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>40121108</v>
       </c>
@@ -10323,7 +10336,7 @@
       <c r="AI52" s="8"/>
       <c r="AJ52" s="8"/>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>40121110</v>
       </c>
@@ -10403,7 +10416,7 @@
       <c r="AI53" s="8"/>
       <c r="AJ53" s="8"/>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:36" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>40121113</v>
       </c>
@@ -10485,7 +10498,7 @@
       <c r="AI54" s="8"/>
       <c r="AJ54" s="8"/>
     </row>
-    <row r="55" spans="1:36" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:36" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>40121119</v>
       </c>
@@ -10569,7 +10582,7 @@
       <c r="AI55" s="8"/>
       <c r="AJ55" s="8"/>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>40121120</v>
       </c>
@@ -10645,7 +10658,7 @@
       <c r="AI56" s="8"/>
       <c r="AJ56" s="8"/>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>40121122</v>
       </c>
@@ -10722,60 +10735,60 @@
       <c r="AI57" s="8"/>
       <c r="AJ57" s="8"/>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="D60" s="131" t="s">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="D60" s="108" t="s">
         <v>80</v>
       </c>
-      <c r="E60" s="132">
+      <c r="E60" s="109">
         <f>C7</f>
         <v>4963678.32</v>
       </c>
-      <c r="H60" s="128"/>
-    </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="D61" s="131" t="s">
+      <c r="H60" s="105"/>
+    </row>
+    <row r="61" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="D61" s="108" t="s">
         <v>81</v>
       </c>
-      <c r="E61" s="133">
+      <c r="E61" s="110">
         <f>SUM(E7:I7)</f>
         <v>1964632.26</v>
       </c>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="D62" s="131" t="s">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="D62" s="108" t="s">
         <v>82</v>
       </c>
-      <c r="E62" s="133">
+      <c r="E62" s="110">
         <f>SUM(J7:P7)</f>
         <v>2859627.79</v>
       </c>
-      <c r="I62" s="128"/>
-      <c r="O62" s="128"/>
-    </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="D63" s="131" t="s">
+      <c r="I62" s="105"/>
+      <c r="O62" s="105"/>
+    </row>
+    <row r="63" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="D63" s="108" t="s">
         <v>83</v>
       </c>
-      <c r="E63" s="134">
+      <c r="E63" s="111">
         <f>E61+E62</f>
         <v>4824260.05</v>
       </c>
-      <c r="H63" s="128"/>
-      <c r="K63" s="128"/>
-      <c r="M63" s="128"/>
-    </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="D64" s="131" t="s">
+      <c r="H63" s="105"/>
+      <c r="K63" s="105"/>
+      <c r="M63" s="105"/>
+    </row>
+    <row r="64" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="D64" s="108" t="s">
         <v>84</v>
       </c>
-      <c r="E64" s="133">
+      <c r="E64" s="110">
         <f>E60-E63</f>
         <v>139418.27000000048</v>
       </c>
-      <c r="H64" s="128"/>
-    </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E70" s="129"/>
+      <c r="H64" s="105"/>
+    </row>
+    <row r="70" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E70" s="106"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -10850,64 +10863,64 @@
       <selection activeCell="D52" sqref="D47:F52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.125" customWidth="1"/>
+    <col min="1" max="1" width="2.09765625" customWidth="1"/>
     <col min="2" max="2" width="47" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="23.625" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="23.59765625" style="31" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" style="32" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.19921875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="1.5" customWidth="1"/>
     <col min="9" max="9" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15.3984375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.625" customWidth="1"/>
-    <col min="15" max="20" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="21" max="30" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.59765625" customWidth="1"/>
+    <col min="15" max="20" width="6.8984375" bestFit="1" customWidth="1"/>
+    <col min="21" max="30" width="7.8984375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="112" t="s">
+    <row r="1" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="120" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="113"/>
-      <c r="M2" s="113"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
       <c r="N2" s="51"/>
     </row>
-    <row r="3" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="114"/>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="115"/>
-      <c r="I3" s="115"/>
-      <c r="J3" s="115"/>
-      <c r="K3" s="115"/>
-      <c r="L3" s="115"/>
-      <c r="M3" s="115"/>
+    <row r="3" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="122"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="123"/>
+      <c r="F3" s="123"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
+      <c r="J3" s="123"/>
+      <c r="K3" s="123"/>
+      <c r="L3" s="123"/>
+      <c r="M3" s="123"/>
       <c r="N3" s="69"/>
     </row>
-    <row r="4" spans="2:14" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B4" s="36"/>
       <c r="N4" s="37"/>
     </row>
-    <row r="5" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="68" t="s">
         <v>61</v>
       </c>
@@ -10916,7 +10929,7 @@
       </c>
       <c r="N5" s="37"/>
     </row>
-    <row r="6" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="38" t="s">
         <v>50</v>
       </c>
@@ -10952,7 +10965,7 @@
       </c>
       <c r="N6" s="37"/>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="43" t="s">
         <v>5</v>
       </c>
@@ -10993,7 +11006,7 @@
       </c>
       <c r="N7" s="37"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="43" t="s">
         <v>5</v>
       </c>
@@ -11034,7 +11047,7 @@
       </c>
       <c r="N8" s="37"/>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="43" t="s">
         <v>5</v>
       </c>
@@ -11074,7 +11087,7 @@
       </c>
       <c r="N9" s="37"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" s="43" t="s">
         <v>9</v>
       </c>
@@ -11115,7 +11128,7 @@
       </c>
       <c r="N10" s="37"/>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="43" t="s">
         <v>11</v>
       </c>
@@ -11156,7 +11169,7 @@
       </c>
       <c r="N11" s="37"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" s="43" t="s">
         <v>11</v>
       </c>
@@ -11197,7 +11210,7 @@
       </c>
       <c r="N12" s="37"/>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" s="43" t="s">
         <v>11</v>
       </c>
@@ -11238,7 +11251,7 @@
       </c>
       <c r="N13" s="37"/>
     </row>
-    <row r="14" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="43" t="s">
         <v>11</v>
       </c>
@@ -11279,7 +11292,7 @@
       </c>
       <c r="N14" s="37"/>
     </row>
-    <row r="15" spans="2:14" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="43" t="s">
         <v>16</v>
       </c>
@@ -11320,7 +11333,7 @@
       </c>
       <c r="N15" s="52"/>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B16" s="43" t="s">
         <v>16</v>
       </c>
@@ -11345,7 +11358,7 @@
       </c>
       <c r="N16" s="37"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="43" t="s">
         <v>19</v>
       </c>
@@ -11373,7 +11386,7 @@
       </c>
       <c r="N17" s="37"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" s="43" t="s">
         <v>19</v>
       </c>
@@ -11396,16 +11409,16 @@
         <f t="shared" si="0"/>
         <v>0.85386102605569847</v>
       </c>
-      <c r="I18" s="110" t="s">
+      <c r="I18" s="118" t="s">
         <v>58</v>
       </c>
-      <c r="J18" s="111"/>
-      <c r="K18" s="111"/>
-      <c r="L18" s="111"/>
-      <c r="M18" s="111"/>
+      <c r="J18" s="119"/>
+      <c r="K18" s="119"/>
+      <c r="L18" s="119"/>
+      <c r="M18" s="119"/>
       <c r="N18" s="37"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" s="43" t="s">
         <v>19</v>
       </c>
@@ -11435,7 +11448,7 @@
       <c r="M19" s="72"/>
       <c r="N19" s="37"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" s="43" t="s">
         <v>19</v>
       </c>
@@ -11475,7 +11488,7 @@
       </c>
       <c r="N20" s="37"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" s="43" t="s">
         <v>19</v>
       </c>
@@ -11519,7 +11532,7 @@
       </c>
       <c r="N21" s="37"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B22" s="43" t="s">
         <v>19</v>
       </c>
@@ -11563,7 +11576,7 @@
       </c>
       <c r="N22" s="37"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" s="43" t="s">
         <v>19</v>
       </c>
@@ -11607,7 +11620,7 @@
       </c>
       <c r="N23" s="37"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" s="43" t="s">
         <v>19</v>
       </c>
@@ -11651,7 +11664,7 @@
       </c>
       <c r="N24" s="37"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" s="43" t="s">
         <v>27</v>
       </c>
@@ -11695,7 +11708,7 @@
       </c>
       <c r="N25" s="37"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" s="43" t="s">
         <v>27</v>
       </c>
@@ -11739,7 +11752,7 @@
       </c>
       <c r="N26" s="37"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B27" s="43" t="s">
         <v>27</v>
       </c>
@@ -11783,7 +11796,7 @@
       </c>
       <c r="N27" s="37"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" s="43" t="s">
         <v>27</v>
       </c>
@@ -11827,7 +11840,7 @@
       </c>
       <c r="N28" s="37"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B29" s="43" t="s">
         <v>27</v>
       </c>
@@ -11871,7 +11884,7 @@
       </c>
       <c r="N29" s="37"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B30" s="43" t="s">
         <v>27</v>
       </c>
@@ -11896,7 +11909,7 @@
       </c>
       <c r="N30" s="37"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B31" s="43" t="s">
         <v>35</v>
       </c>
@@ -11921,7 +11934,7 @@
       </c>
       <c r="N31" s="53"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B32" s="43" t="s">
         <v>37</v>
       </c>
@@ -11946,7 +11959,7 @@
       </c>
       <c r="N32" s="37"/>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B33" s="43" t="s">
         <v>37</v>
       </c>
@@ -11971,7 +11984,7 @@
       </c>
       <c r="N33" s="37"/>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B34" s="43" t="s">
         <v>37</v>
       </c>
@@ -11994,16 +12007,16 @@
         <f t="shared" si="0"/>
         <v>0.91116350589441319</v>
       </c>
-      <c r="I34" s="118" t="s">
+      <c r="I34" s="126" t="s">
         <v>63</v>
       </c>
-      <c r="J34" s="119"/>
-      <c r="K34" s="119"/>
-      <c r="L34" s="119"/>
-      <c r="M34" s="120"/>
+      <c r="J34" s="127"/>
+      <c r="K34" s="127"/>
+      <c r="L34" s="127"/>
+      <c r="M34" s="128"/>
       <c r="N34" s="37"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B35" s="43" t="s">
         <v>37</v>
       </c>
@@ -12026,14 +12039,14 @@
         <f t="shared" si="0"/>
         <v>0.66542666666666661</v>
       </c>
-      <c r="I35" s="121"/>
-      <c r="J35" s="122"/>
-      <c r="K35" s="122"/>
-      <c r="L35" s="122"/>
-      <c r="M35" s="123"/>
+      <c r="I35" s="129"/>
+      <c r="J35" s="130"/>
+      <c r="K35" s="130"/>
+      <c r="L35" s="130"/>
+      <c r="M35" s="131"/>
       <c r="N35" s="37"/>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B36" s="43" t="s">
         <v>37</v>
       </c>
@@ -12056,14 +12069,14 @@
         <f t="shared" si="0"/>
         <v>0.80938352865628505</v>
       </c>
-      <c r="I36" s="121"/>
-      <c r="J36" s="122"/>
-      <c r="K36" s="122"/>
-      <c r="L36" s="122"/>
-      <c r="M36" s="123"/>
+      <c r="I36" s="129"/>
+      <c r="J36" s="130"/>
+      <c r="K36" s="130"/>
+      <c r="L36" s="130"/>
+      <c r="M36" s="131"/>
       <c r="N36" s="37"/>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B37" s="43" t="s">
         <v>37</v>
       </c>
@@ -12086,14 +12099,14 @@
         <f t="shared" si="0"/>
         <v>100%</v>
       </c>
-      <c r="I37" s="121"/>
-      <c r="J37" s="122"/>
-      <c r="K37" s="122"/>
-      <c r="L37" s="122"/>
-      <c r="M37" s="123"/>
+      <c r="I37" s="129"/>
+      <c r="J37" s="130"/>
+      <c r="K37" s="130"/>
+      <c r="L37" s="130"/>
+      <c r="M37" s="131"/>
       <c r="N37" s="37"/>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B38" s="43" t="s">
         <v>37</v>
       </c>
@@ -12116,14 +12129,14 @@
         <f t="shared" si="0"/>
         <v>1.1139522606250856</v>
       </c>
-      <c r="I38" s="121"/>
-      <c r="J38" s="122"/>
-      <c r="K38" s="122"/>
-      <c r="L38" s="122"/>
-      <c r="M38" s="123"/>
+      <c r="I38" s="129"/>
+      <c r="J38" s="130"/>
+      <c r="K38" s="130"/>
+      <c r="L38" s="130"/>
+      <c r="M38" s="131"/>
       <c r="N38" s="37"/>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B39" s="43" t="s">
         <v>37</v>
       </c>
@@ -12146,14 +12159,14 @@
         <f t="shared" si="0"/>
         <v>0.71851149999999997</v>
       </c>
-      <c r="I39" s="121"/>
-      <c r="J39" s="122"/>
-      <c r="K39" s="122"/>
-      <c r="L39" s="122"/>
-      <c r="M39" s="123"/>
+      <c r="I39" s="129"/>
+      <c r="J39" s="130"/>
+      <c r="K39" s="130"/>
+      <c r="L39" s="130"/>
+      <c r="M39" s="131"/>
       <c r="N39" s="37"/>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B40" s="59" t="s">
         <v>37</v>
       </c>
@@ -12176,18 +12189,18 @@
         <f t="shared" si="0"/>
         <v>100%</v>
       </c>
-      <c r="I40" s="121"/>
-      <c r="J40" s="122"/>
-      <c r="K40" s="122"/>
-      <c r="L40" s="122"/>
-      <c r="M40" s="123"/>
+      <c r="I40" s="129"/>
+      <c r="J40" s="130"/>
+      <c r="K40" s="130"/>
+      <c r="L40" s="130"/>
+      <c r="M40" s="131"/>
       <c r="N40" s="70"/>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B41" s="116" t="s">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B41" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="117"/>
+      <c r="C41" s="125"/>
       <c r="D41" s="64">
         <f>SUM(D7:D40)</f>
         <v>4963678.32</v>
@@ -12205,14 +12218,14 @@
         <v>0.97191230756468527</v>
       </c>
       <c r="H41" s="58"/>
-      <c r="I41" s="124"/>
-      <c r="J41" s="125"/>
-      <c r="K41" s="125"/>
-      <c r="L41" s="125"/>
-      <c r="M41" s="126"/>
+      <c r="I41" s="132"/>
+      <c r="J41" s="133"/>
+      <c r="K41" s="133"/>
+      <c r="L41" s="133"/>
+      <c r="M41" s="134"/>
       <c r="N41" s="70"/>
     </row>
-    <row r="42" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B42" s="55"/>
       <c r="C42" s="44"/>
       <c r="D42" s="56"/>
@@ -12227,14 +12240,14 @@
       <c r="M42" s="44"/>
       <c r="N42" s="54"/>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D48" s="130"/>
-    </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E49" s="130"/>
-    </row>
-    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D51" s="130"/>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D48" s="107"/>
+    </row>
+    <row r="49" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E49" s="107"/>
+    </row>
+    <row r="51" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D51" s="107"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -12320,37 +12333,37 @@
       <selection activeCell="G4" sqref="G4:K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.875" customWidth="1"/>
-    <col min="4" max="5" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.8984375" customWidth="1"/>
+    <col min="4" max="5" width="11.09765625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="18" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.25" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.8984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="18" width="13.8984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.19921875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.09765625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.3984375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.19921875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.09765625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.19921875" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="8" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.09765625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="8" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.75" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.69921875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.09765625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="93" t="s">
         <v>70</v>
       </c>
@@ -12364,7 +12377,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="95" t="s">
         <v>71</v>
       </c>
@@ -12384,7 +12397,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="95" t="s">
         <v>71</v>
       </c>
@@ -12443,7 +12456,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="95" t="s">
         <v>71</v>
       </c>
@@ -12503,7 +12516,7 @@
         <v>7035.1196640083326</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="95" t="s">
         <v>71</v>
       </c>
@@ -12563,7 +12576,7 @@
         <v>58333.333333333328</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="95" t="s">
         <v>71</v>
       </c>
@@ -12623,7 +12636,7 @@
         <v>4325.8333333333339</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="95" t="s">
         <v>71</v>
       </c>
@@ -12683,7 +12696,7 @@
         <v>115000</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="95" t="s">
         <v>71</v>
       </c>
@@ -12743,7 +12756,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="95" t="s">
         <v>71</v>
       </c>
@@ -12803,7 +12816,7 @@
         <v>98748.880524707332</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="95" t="s">
         <v>71</v>
       </c>
@@ -12863,7 +12876,7 @@
         <v>97443.337847222225</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="95" t="s">
         <v>71</v>
       </c>
@@ -12923,7 +12936,7 @@
         <v>104166.66666666666</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="95" t="s">
         <v>71</v>
       </c>
@@ -12983,7 +12996,7 @@
         <v>7465.6962000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="95" t="s">
         <v>71</v>
       </c>
@@ -13043,7 +13056,7 @@
         <v>41666.666666666672</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="95" t="s">
         <v>71</v>
       </c>
@@ -13103,7 +13116,7 @@
         <v>434901.83333333337</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="95" t="s">
         <v>71</v>
       </c>
@@ -13163,7 +13176,7 @@
         <v>83333.333333333343</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="95" t="s">
         <v>71</v>
       </c>
@@ -13223,7 +13236,7 @@
         <v>41666.666666666672</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="95" t="s">
         <v>71</v>
       </c>
@@ -13283,7 +13296,7 @@
         <v>1685.3446666666669</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="95" t="s">
         <v>71</v>
       </c>
@@ -13343,7 +13356,7 @@
         <v>8651.6666666666679</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="95" t="s">
         <v>71</v>
       </c>
@@ -13403,7 +13416,7 @@
         <v>166666.66666666669</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="95" t="s">
         <v>71</v>
       </c>
@@ -13463,7 +13476,7 @@
         <v>8651.6666666666679</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="95" t="s">
         <v>71</v>
       </c>
@@ -13523,7 +13536,7 @@
         <v>4166.666666666667</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="95" t="s">
         <v>71</v>
       </c>
@@ -13583,7 +13596,7 @@
         <v>3071.3416666666667</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="98" t="s">
         <v>72</v>
       </c>
@@ -13643,7 +13656,7 @@
         <v>467.18999999999994</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="98" t="s">
         <v>72</v>
       </c>
@@ -13703,7 +13716,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="98" t="s">
         <v>72</v>
       </c>
@@ -13763,7 +13776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="98" t="s">
         <v>72</v>
       </c>
@@ -13823,7 +13836,7 @@
         <v>310330.91110666667</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="98" t="s">
         <v>72</v>
       </c>
@@ -13883,7 +13896,7 @@
         <v>41666.666666666657</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="98" t="s">
         <v>72</v>
       </c>
@@ -13939,7 +13952,7 @@
         <v>4963678.6716222521</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="98" t="s">
         <v>72</v>
       </c>
@@ -13953,7 +13966,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="98" t="s">
         <v>72</v>
       </c>
@@ -13967,7 +13980,7 @@
         <v>5833.333333333333</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="95" t="s">
         <v>71</v>
       </c>
@@ -13981,7 +13994,7 @@
         <v>1407.0239328016664</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="95" t="s">
         <v>71</v>
       </c>
@@ -13995,7 +14008,7 @@
         <v>11666.666666666666</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="95" t="s">
         <v>71</v>
       </c>
@@ -14009,7 +14022,7 @@
         <v>865.16666666666674</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="95" t="s">
         <v>71</v>
       </c>
@@ -14023,7 +14036,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="95" t="s">
         <v>71</v>
       </c>
@@ -14037,7 +14050,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="95" t="s">
         <v>71</v>
       </c>
@@ -14051,7 +14064,7 @@
         <v>19749.776104941466</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="95" t="s">
         <v>71</v>
       </c>
@@ -14065,7 +14078,7 @@
         <v>19488.667569444446</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="95" t="s">
         <v>71</v>
       </c>
@@ -14079,7 +14092,7 @@
         <v>20833.333333333332</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="95" t="s">
         <v>71</v>
       </c>
@@ -14093,7 +14106,7 @@
         <v>1493.13924</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="95" t="s">
         <v>71</v>
       </c>
@@ -14107,7 +14120,7 @@
         <v>11277.666666666666</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="95" t="s">
         <v>71</v>
       </c>
@@ -14121,7 +14134,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="95" t="s">
         <v>71</v>
       </c>
@@ -14135,7 +14148,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="95" t="s">
         <v>71</v>
       </c>
@@ -14149,7 +14162,7 @@
         <v>337.06893333333335</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="95" t="s">
         <v>71</v>
       </c>
@@ -14163,7 +14176,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="95" t="s">
         <v>71</v>
       </c>
@@ -14177,7 +14190,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="95" t="s">
         <v>71</v>
       </c>
@@ -14191,7 +14204,7 @@
         <v>833.33333333333337</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="95" t="s">
         <v>71</v>
       </c>
@@ -14205,7 +14218,7 @@
         <v>614.26833333333332</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="95" t="s">
         <v>71</v>
       </c>
@@ -14219,7 +14232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="95" t="s">
         <v>71</v>
       </c>
@@ -14233,7 +14246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="95" t="s">
         <v>71</v>
       </c>
@@ -14247,7 +14260,7 @@
         <v>30908.863333333331</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="95" t="s">
         <v>71</v>
       </c>
@@ -14261,7 +14274,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="98" t="s">
         <v>72</v>
       </c>
@@ -14275,7 +14288,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="98" t="s">
         <v>72</v>
       </c>
@@ -14289,7 +14302,7 @@
         <v>75702.7</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="98" t="s">
         <v>72</v>
       </c>
@@ -14303,7 +14316,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="98" t="s">
         <v>72</v>
       </c>
@@ -14317,7 +14330,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="98" t="s">
         <v>72</v>
       </c>
@@ -14331,7 +14344,7 @@
         <v>31157.318887999998</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="98" t="s">
         <v>72</v>
       </c>
@@ -14345,7 +14358,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="98" t="s">
         <v>72</v>
       </c>
@@ -14359,7 +14372,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="98" t="s">
         <v>72</v>
       </c>
@@ -14373,7 +14386,7 @@
         <v>5833.333333333333</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="95" t="s">
         <v>71</v>
       </c>
@@ -14387,7 +14400,7 @@
         <v>1407.0239328016664</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="95" t="s">
         <v>71</v>
       </c>
@@ -14401,7 +14414,7 @@
         <v>11666.666666666666</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="95" t="s">
         <v>71</v>
       </c>
@@ -14415,7 +14428,7 @@
         <v>865.16666666666674</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="95" t="s">
         <v>71</v>
       </c>
@@ -14429,7 +14442,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="95" t="s">
         <v>71</v>
       </c>
@@ -14443,7 +14456,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="95" t="s">
         <v>71</v>
       </c>
@@ -14457,7 +14470,7 @@
         <v>19749.776104941466</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="95" t="s">
         <v>71</v>
       </c>
@@ -14471,7 +14484,7 @@
         <v>19488.667569444446</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="95" t="s">
         <v>71</v>
       </c>
@@ -14485,7 +14498,7 @@
         <v>20833.333333333332</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="95" t="s">
         <v>71</v>
       </c>
@@ -14499,7 +14512,7 @@
         <v>1493.13924</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="95" t="s">
         <v>71</v>
       </c>
@@ -14513,7 +14526,7 @@
         <v>11277.666666666666</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="95" t="s">
         <v>71</v>
       </c>
@@ -14527,7 +14540,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="95" t="s">
         <v>71</v>
       </c>
@@ -14541,7 +14554,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="95" t="s">
         <v>71</v>
       </c>
@@ -14555,7 +14568,7 @@
         <v>337.06893333333335</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="95" t="s">
         <v>71</v>
       </c>
@@ -14569,7 +14582,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="95" t="s">
         <v>71</v>
       </c>
@@ -14583,7 +14596,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="95" t="s">
         <v>71</v>
       </c>
@@ -14597,7 +14610,7 @@
         <v>833.33333333333337</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="95" t="s">
         <v>71</v>
       </c>
@@ -14611,7 +14624,7 @@
         <v>614.26833333333332</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="95" t="s">
         <v>71</v>
       </c>
@@ -14625,7 +14638,7 @@
         <v>155.72999999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="95" t="s">
         <v>71</v>
       </c>
@@ -14639,7 +14652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="95" t="s">
         <v>71</v>
       </c>
@@ -14653,7 +14666,7 @@
         <v>30908.863333333331</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="95" t="s">
         <v>71</v>
       </c>
@@ -14667,7 +14680,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="98" t="s">
         <v>72</v>
       </c>
@@ -14681,7 +14694,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="98" t="s">
         <v>72</v>
       </c>
@@ -14695,7 +14708,7 @@
         <v>75702.7</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="98" t="s">
         <v>72</v>
       </c>
@@ -14709,7 +14722,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="98" t="s">
         <v>72</v>
       </c>
@@ -14723,7 +14736,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="98" t="s">
         <v>72</v>
       </c>
@@ -14737,7 +14750,7 @@
         <v>31157.318887999998</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="98" t="s">
         <v>72</v>
       </c>
@@ -14751,7 +14764,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="98" t="s">
         <v>72</v>
       </c>
@@ -14765,7 +14778,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="98" t="s">
         <v>72</v>
       </c>
@@ -14779,7 +14792,7 @@
         <v>5833.333333333333</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="95" t="s">
         <v>71</v>
       </c>
@@ -14793,7 +14806,7 @@
         <v>1407.0239328016664</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="95" t="s">
         <v>71</v>
       </c>
@@ -14807,7 +14820,7 @@
         <v>11666.666666666666</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="95" t="s">
         <v>71</v>
       </c>
@@ -14821,7 +14834,7 @@
         <v>865.16666666666674</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="95" t="s">
         <v>71</v>
       </c>
@@ -14835,7 +14848,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="95" t="s">
         <v>71</v>
       </c>
@@ -14849,7 +14862,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="95" t="s">
         <v>71</v>
       </c>
@@ -14863,7 +14876,7 @@
         <v>19749.776104941466</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="95" t="s">
         <v>71</v>
       </c>
@@ -14877,7 +14890,7 @@
         <v>19488.667569444446</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="95" t="s">
         <v>71</v>
       </c>
@@ -14891,7 +14904,7 @@
         <v>20833.333333333332</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="95" t="s">
         <v>71</v>
       </c>
@@ -14905,7 +14918,7 @@
         <v>1493.13924</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="95" t="s">
         <v>71</v>
       </c>
@@ -14919,7 +14932,7 @@
         <v>11277.666666666666</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="95" t="s">
         <v>71</v>
       </c>
@@ -14933,7 +14946,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="95" t="s">
         <v>71</v>
       </c>
@@ -14947,7 +14960,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="95" t="s">
         <v>71</v>
       </c>
@@ -14961,7 +14974,7 @@
         <v>337.06893333333335</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="95" t="s">
         <v>71</v>
       </c>
@@ -14975,7 +14988,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="95" t="s">
         <v>71</v>
       </c>
@@ -14989,7 +15002,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="95" t="s">
         <v>71</v>
       </c>
@@ -15003,7 +15016,7 @@
         <v>833.33333333333337</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="95" t="s">
         <v>71</v>
       </c>
@@ -15017,7 +15030,7 @@
         <v>614.26833333333332</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="95" t="s">
         <v>71</v>
       </c>
@@ -15031,7 +15044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="95" t="s">
         <v>71</v>
       </c>
@@ -15045,7 +15058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="95" t="s">
         <v>71</v>
       </c>
@@ -15059,7 +15072,7 @@
         <v>30908.863333333331</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="95" t="s">
         <v>71</v>
       </c>
@@ -15073,7 +15086,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="98" t="s">
         <v>72</v>
       </c>
@@ -15087,7 +15100,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="98" t="s">
         <v>72</v>
       </c>
@@ -15101,7 +15114,7 @@
         <v>75702.7</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="98" t="s">
         <v>72</v>
       </c>
@@ -15115,7 +15128,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="98" t="s">
         <v>72</v>
       </c>
@@ -15129,7 +15142,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="98" t="s">
         <v>72</v>
       </c>
@@ -15143,7 +15156,7 @@
         <v>31157.318887999998</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="98" t="s">
         <v>72</v>
       </c>
@@ -15157,7 +15170,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="98" t="s">
         <v>72</v>
       </c>
@@ -15171,7 +15184,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="98" t="s">
         <v>72</v>
       </c>
@@ -15185,7 +15198,7 @@
         <v>5833.333333333333</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="95" t="s">
         <v>71</v>
       </c>
@@ -15199,7 +15212,7 @@
         <v>1407.0239328016664</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="95" t="s">
         <v>71</v>
       </c>
@@ -15213,7 +15226,7 @@
         <v>11666.666666666666</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="95" t="s">
         <v>71</v>
       </c>
@@ -15227,7 +15240,7 @@
         <v>865.16666666666674</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="95" t="s">
         <v>71</v>
       </c>
@@ -15241,7 +15254,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="95" t="s">
         <v>71</v>
       </c>
@@ -15255,7 +15268,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="95" t="s">
         <v>71</v>
       </c>
@@ -15269,7 +15282,7 @@
         <v>19749.776104941466</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="95" t="s">
         <v>71</v>
       </c>
@@ -15283,7 +15296,7 @@
         <v>19488.667569444446</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="95" t="s">
         <v>71</v>
       </c>
@@ -15297,7 +15310,7 @@
         <v>20833.333333333332</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="95" t="s">
         <v>71</v>
       </c>
@@ -15311,7 +15324,7 @@
         <v>1493.13924</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="95" t="s">
         <v>71</v>
       </c>
@@ -15325,7 +15338,7 @@
         <v>11277.666666666666</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="95" t="s">
         <v>71</v>
       </c>
@@ -15339,7 +15352,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="95" t="s">
         <v>71</v>
       </c>
@@ -15353,7 +15366,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="95" t="s">
         <v>71</v>
       </c>
@@ -15367,7 +15380,7 @@
         <v>337.06893333333335</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="95" t="s">
         <v>71</v>
       </c>
@@ -15381,7 +15394,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="95" t="s">
         <v>71</v>
       </c>
@@ -15395,7 +15408,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="95" t="s">
         <v>71</v>
       </c>
@@ -15409,7 +15422,7 @@
         <v>833.33333333333337</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="95" t="s">
         <v>71</v>
       </c>
@@ -15423,7 +15436,7 @@
         <v>614.26833333333332</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="95" t="s">
         <v>71</v>
       </c>
@@ -15437,7 +15450,7 @@
         <v>155.72999999999999</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="95" t="s">
         <v>71</v>
       </c>
@@ -15451,7 +15464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="95" t="s">
         <v>71</v>
       </c>
@@ -15465,7 +15478,7 @@
         <v>30908.863333333331</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="95" t="s">
         <v>71</v>
       </c>
@@ -15479,7 +15492,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="98" t="s">
         <v>72</v>
       </c>
@@ -15493,7 +15506,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="98" t="s">
         <v>72</v>
       </c>
@@ -15507,7 +15520,7 @@
         <v>75702.7</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="98" t="s">
         <v>72</v>
       </c>
@@ -15521,7 +15534,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="98" t="s">
         <v>72</v>
       </c>
@@ -15535,7 +15548,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="98" t="s">
         <v>72</v>
       </c>
@@ -15549,7 +15562,7 @@
         <v>31157.318887999998</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="98" t="s">
         <v>72</v>
       </c>
@@ -15563,7 +15576,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="98" t="s">
         <v>72</v>
       </c>
@@ -15577,7 +15590,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="98" t="s">
         <v>72</v>
       </c>
@@ -15591,7 +15604,7 @@
         <v>5833.333333333333</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="95" t="s">
         <v>71</v>
       </c>
@@ -15605,7 +15618,7 @@
         <v>1407.0239328016664</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="95" t="s">
         <v>71</v>
       </c>
@@ -15619,7 +15632,7 @@
         <v>11666.666666666666</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="95" t="s">
         <v>71</v>
       </c>
@@ -15633,7 +15646,7 @@
         <v>865.16666666666674</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="95" t="s">
         <v>71</v>
       </c>
@@ -15647,7 +15660,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="95" t="s">
         <v>71</v>
       </c>
@@ -15661,7 +15674,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="95" t="s">
         <v>71</v>
       </c>
@@ -15675,7 +15688,7 @@
         <v>19749.776104941466</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="95" t="s">
         <v>71</v>
       </c>
@@ -15689,7 +15702,7 @@
         <v>19488.667569444446</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="95" t="s">
         <v>71</v>
       </c>
@@ -15703,7 +15716,7 @@
         <v>20833.333333333332</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="95" t="s">
         <v>71</v>
       </c>
@@ -15717,7 +15730,7 @@
         <v>1493.13924</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="95" t="s">
         <v>71</v>
       </c>
@@ -15731,7 +15744,7 @@
         <v>11277.666666666666</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="95" t="s">
         <v>71</v>
       </c>
@@ -15745,7 +15758,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="95" t="s">
         <v>71</v>
       </c>
@@ -15759,7 +15772,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="95" t="s">
         <v>71</v>
       </c>
@@ -15773,7 +15786,7 @@
         <v>337.06893333333335</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" s="95" t="s">
         <v>71</v>
       </c>
@@ -15787,7 +15800,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" s="95" t="s">
         <v>71</v>
       </c>
@@ -15801,7 +15814,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" s="95" t="s">
         <v>71</v>
       </c>
@@ -15815,7 +15828,7 @@
         <v>833.33333333333337</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" s="95" t="s">
         <v>71</v>
       </c>
@@ -15829,7 +15842,7 @@
         <v>614.26833333333332</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" s="95" t="s">
         <v>71</v>
       </c>
@@ -15843,7 +15856,7 @@
         <v>1483.5878</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" s="95" t="s">
         <v>71</v>
       </c>
@@ -15857,7 +15870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" s="95" t="s">
         <v>71</v>
       </c>
@@ -15871,7 +15884,7 @@
         <v>30908.863333333331</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" s="95" t="s">
         <v>71</v>
       </c>
@@ -15885,7 +15898,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" s="98" t="s">
         <v>72</v>
       </c>
@@ -15899,7 +15912,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" s="98" t="s">
         <v>72</v>
       </c>
@@ -15913,7 +15926,7 @@
         <v>75702.7</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" s="98" t="s">
         <v>72</v>
       </c>
@@ -15927,7 +15940,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" s="98" t="s">
         <v>72</v>
       </c>
@@ -15941,7 +15954,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" s="98" t="s">
         <v>72</v>
       </c>
@@ -15955,7 +15968,7 @@
         <v>31157.318887999998</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" s="98" t="s">
         <v>72</v>
       </c>
@@ -15969,7 +15982,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" s="98" t="s">
         <v>72</v>
       </c>
@@ -15983,7 +15996,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" s="98" t="s">
         <v>72</v>
       </c>
@@ -15997,7 +16010,7 @@
         <v>5833.333333333333</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" s="95" t="s">
         <v>71</v>
       </c>
@@ -16011,7 +16024,7 @@
         <v>1407.0239328016664</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" s="95" t="s">
         <v>71</v>
       </c>
@@ -16025,7 +16038,7 @@
         <v>11666.666666666666</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" s="95" t="s">
         <v>71</v>
       </c>
@@ -16039,7 +16052,7 @@
         <v>865.16666666666674</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" s="95" t="s">
         <v>71</v>
       </c>
@@ -16053,7 +16066,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" s="95" t="s">
         <v>71</v>
       </c>
@@ -16067,7 +16080,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" s="95" t="s">
         <v>71</v>
       </c>
@@ -16081,7 +16094,7 @@
         <v>19749.776104941466</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" s="95" t="s">
         <v>71</v>
       </c>
@@ -16095,7 +16108,7 @@
         <v>19488.667569444446</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="95" t="s">
         <v>71</v>
       </c>
@@ -16109,7 +16122,7 @@
         <v>20833.333333333332</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" s="95" t="s">
         <v>71</v>
       </c>
@@ -16123,7 +16136,7 @@
         <v>1493.13924</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" s="95" t="s">
         <v>71</v>
       </c>
@@ -16137,7 +16150,7 @@
         <v>11277.666666666666</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" s="95" t="s">
         <v>71</v>
       </c>
@@ -16151,7 +16164,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" s="95" t="s">
         <v>71</v>
       </c>
@@ -16165,7 +16178,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" s="95" t="s">
         <v>71</v>
       </c>
@@ -16179,7 +16192,7 @@
         <v>337.06893333333335</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" s="95" t="s">
         <v>71</v>
       </c>
@@ -16193,7 +16206,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" s="95" t="s">
         <v>71</v>
       </c>
@@ -16207,7 +16220,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" s="95" t="s">
         <v>71</v>
       </c>
@@ -16221,7 +16234,7 @@
         <v>833.33333333333337</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" s="95" t="s">
         <v>71</v>
       </c>
@@ -16235,7 +16248,7 @@
         <v>614.26833333333332</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" s="95" t="s">
         <v>71</v>
       </c>
@@ -16249,7 +16262,7 @@
         <v>155.72999999999999</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" s="95" t="s">
         <v>71</v>
       </c>
@@ -16263,7 +16276,7 @@
         <v>6229.2</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" s="95" t="s">
         <v>71</v>
       </c>
@@ -16277,7 +16290,7 @@
         <v>30908.863333333331</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" s="95" t="s">
         <v>71</v>
       </c>
@@ -16291,7 +16304,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" s="98" t="s">
         <v>72</v>
       </c>
@@ -16305,7 +16318,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" s="98" t="s">
         <v>72</v>
       </c>
@@ -16319,7 +16332,7 @@
         <v>75702.7</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" s="98" t="s">
         <v>72</v>
       </c>
@@ -16333,7 +16346,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" s="98" t="s">
         <v>72</v>
       </c>
@@ -16347,7 +16360,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" s="98" t="s">
         <v>72</v>
       </c>
@@ -16361,7 +16374,7 @@
         <v>31157.318887999998</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" s="98" t="s">
         <v>72</v>
       </c>
@@ -16375,7 +16388,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" s="98" t="s">
         <v>72</v>
       </c>
@@ -16389,7 +16402,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" s="98" t="s">
         <v>72</v>
       </c>
@@ -16403,7 +16416,7 @@
         <v>5833.333333333333</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" s="95" t="s">
         <v>71</v>
       </c>
@@ -16417,7 +16430,7 @@
         <v>1407.0239328016664</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" s="95" t="s">
         <v>71</v>
       </c>
@@ -16431,7 +16444,7 @@
         <v>11666.666666666666</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" s="95" t="s">
         <v>71</v>
       </c>
@@ -16445,7 +16458,7 @@
         <v>865.16666666666674</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" s="95" t="s">
         <v>71</v>
       </c>
@@ -16459,7 +16472,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" s="95" t="s">
         <v>71</v>
       </c>
@@ -16473,7 +16486,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" s="95" t="s">
         <v>71</v>
       </c>
@@ -16487,7 +16500,7 @@
         <v>19749.776104941466</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" s="95" t="s">
         <v>71</v>
       </c>
@@ -16501,7 +16514,7 @@
         <v>19488.667569444446</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" s="95" t="s">
         <v>71</v>
       </c>
@@ -16515,7 +16528,7 @@
         <v>20833.333333333332</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" s="95" t="s">
         <v>71</v>
       </c>
@@ -16529,7 +16542,7 @@
         <v>1493.13924</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" s="95" t="s">
         <v>71</v>
       </c>
@@ -16543,7 +16556,7 @@
         <v>11277.666666666666</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" s="95" t="s">
         <v>71</v>
       </c>
@@ -16557,7 +16570,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" s="95" t="s">
         <v>71</v>
       </c>
@@ -16571,7 +16584,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" s="95" t="s">
         <v>71</v>
       </c>
@@ -16585,7 +16598,7 @@
         <v>337.06893333333335</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" s="95" t="s">
         <v>71</v>
       </c>
@@ -16599,7 +16612,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" s="95" t="s">
         <v>71</v>
       </c>
@@ -16613,7 +16626,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" s="95" t="s">
         <v>71</v>
       </c>
@@ -16627,7 +16640,7 @@
         <v>833.33333333333337</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" s="95" t="s">
         <v>71</v>
       </c>
@@ -16641,7 +16654,7 @@
         <v>614.26833333333332</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" s="95" t="s">
         <v>71</v>
       </c>
@@ -16655,7 +16668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" s="95" t="s">
         <v>71</v>
       </c>
@@ -16669,7 +16682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" s="95" t="s">
         <v>71</v>
       </c>
@@ -16683,7 +16696,7 @@
         <v>30908.863333333331</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" s="95" t="s">
         <v>71</v>
       </c>
@@ -16697,7 +16710,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" s="98" t="s">
         <v>72</v>
       </c>
@@ -16711,7 +16724,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" s="98" t="s">
         <v>72</v>
       </c>
@@ -16725,7 +16738,7 @@
         <v>75702.7</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" s="98" t="s">
         <v>72</v>
       </c>
@@ -16739,7 +16752,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" s="98" t="s">
         <v>72</v>
       </c>
@@ -16753,7 +16766,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" s="98" t="s">
         <v>72</v>
       </c>
@@ -16767,7 +16780,7 @@
         <v>31157.318887999998</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" s="98" t="s">
         <v>72</v>
       </c>
@@ -16781,7 +16794,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" s="98" t="s">
         <v>72</v>
       </c>
@@ -16795,7 +16808,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" s="98" t="s">
         <v>72</v>
       </c>
@@ -16809,7 +16822,7 @@
         <v>5833.333333333333</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" s="95" t="s">
         <v>71</v>
       </c>
@@ -16823,7 +16836,7 @@
         <v>1407.0239328016664</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" s="95" t="s">
         <v>71</v>
       </c>
@@ -16837,7 +16850,7 @@
         <v>11666.666666666666</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" s="95" t="s">
         <v>71</v>
       </c>
@@ -16851,7 +16864,7 @@
         <v>865.16666666666674</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" s="95" t="s">
         <v>71</v>
       </c>
@@ -16865,7 +16878,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" s="95" t="s">
         <v>71</v>
       </c>
@@ -16879,7 +16892,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" s="95" t="s">
         <v>71</v>
       </c>
@@ -16893,7 +16906,7 @@
         <v>19749.776104941466</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" s="95" t="s">
         <v>71</v>
       </c>
@@ -16907,7 +16920,7 @@
         <v>19488.667569444446</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" s="95" t="s">
         <v>71</v>
       </c>
@@ -16921,7 +16934,7 @@
         <v>20833.333333333332</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" s="95" t="s">
         <v>71</v>
       </c>
@@ -16935,7 +16948,7 @@
         <v>1493.13924</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243" s="95" t="s">
         <v>71</v>
       </c>
@@ -16949,7 +16962,7 @@
         <v>11277.666666666666</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244" s="95" t="s">
         <v>71</v>
       </c>
@@ -16963,7 +16976,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245" s="95" t="s">
         <v>71</v>
       </c>
@@ -16977,7 +16990,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246" s="95" t="s">
         <v>71</v>
       </c>
@@ -16991,7 +17004,7 @@
         <v>337.06893333333335</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247" s="95" t="s">
         <v>71</v>
       </c>
@@ -17005,7 +17018,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A248" s="95" t="s">
         <v>71</v>
       </c>
@@ -17019,7 +17032,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A249" s="95" t="s">
         <v>71</v>
       </c>
@@ -17033,7 +17046,7 @@
         <v>833.33333333333337</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A250" s="95" t="s">
         <v>71</v>
       </c>
@@ -17047,7 +17060,7 @@
         <v>614.26833333333332</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A251" s="95" t="s">
         <v>71</v>
       </c>
@@ -17061,7 +17074,7 @@
         <v>155.72999999999999</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A252" s="95" t="s">
         <v>71</v>
       </c>
@@ -17075,7 +17088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A253" s="95" t="s">
         <v>71</v>
       </c>
@@ -17089,7 +17102,7 @@
         <v>30908.863333333331</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A254" s="95" t="s">
         <v>71</v>
       </c>
@@ -17103,7 +17116,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A255" s="98" t="s">
         <v>72</v>
       </c>
@@ -17117,7 +17130,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A256" s="98" t="s">
         <v>72</v>
       </c>
@@ -17131,7 +17144,7 @@
         <v>75702.7</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A257" s="98" t="s">
         <v>72</v>
       </c>
@@ -17145,7 +17158,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A258" s="98" t="s">
         <v>72</v>
       </c>
@@ -17159,7 +17172,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A259" s="98" t="s">
         <v>72</v>
       </c>
@@ -17173,7 +17186,7 @@
         <v>31157.318887999998</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A260" s="98" t="s">
         <v>72</v>
       </c>
@@ -17187,7 +17200,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A261" s="98" t="s">
         <v>72</v>
       </c>
@@ -17201,7 +17214,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A262" s="98" t="s">
         <v>72</v>
       </c>
@@ -17215,7 +17228,7 @@
         <v>5833.333333333333</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A263" s="95" t="s">
         <v>71</v>
       </c>
@@ -17229,7 +17242,7 @@
         <v>1407.0239328016664</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A264" s="95" t="s">
         <v>71</v>
       </c>
@@ -17243,7 +17256,7 @@
         <v>11666.666666666666</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A265" s="95" t="s">
         <v>71</v>
       </c>
@@ -17257,7 +17270,7 @@
         <v>865.16666666666674</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A266" s="95" t="s">
         <v>71</v>
       </c>
@@ -17271,7 +17284,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A267" s="95" t="s">
         <v>71</v>
       </c>
@@ -17285,7 +17298,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A268" s="95" t="s">
         <v>71</v>
       </c>
@@ -17299,7 +17312,7 @@
         <v>19749.776104941466</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A269" s="95" t="s">
         <v>71</v>
       </c>
@@ -17313,7 +17326,7 @@
         <v>19488.667569444446</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A270" s="95" t="s">
         <v>71</v>
       </c>
@@ -17327,7 +17340,7 @@
         <v>20833.333333333332</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A271" s="95" t="s">
         <v>71</v>
       </c>
@@ -17341,7 +17354,7 @@
         <v>1493.13924</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A272" s="95" t="s">
         <v>71</v>
       </c>
@@ -17355,7 +17368,7 @@
         <v>11277.666666666666</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A273" s="95" t="s">
         <v>71</v>
       </c>
@@ -17369,7 +17382,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A274" s="95" t="s">
         <v>71</v>
       </c>
@@ -17383,7 +17396,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A275" s="95" t="s">
         <v>71</v>
       </c>
@@ -17397,7 +17410,7 @@
         <v>337.06893333333335</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A276" s="95" t="s">
         <v>71</v>
       </c>
@@ -17411,7 +17424,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A277" s="95" t="s">
         <v>71</v>
       </c>
@@ -17425,7 +17438,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A278" s="95" t="s">
         <v>71</v>
       </c>
@@ -17439,7 +17452,7 @@
         <v>833.33333333333337</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A279" s="95" t="s">
         <v>71</v>
       </c>
@@ -17453,7 +17466,7 @@
         <v>614.26833333333332</v>
       </c>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A280" s="95" t="s">
         <v>71</v>
       </c>
@@ -17467,7 +17480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A281" s="95" t="s">
         <v>71</v>
       </c>
@@ -17481,7 +17494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A282" s="95" t="s">
         <v>71</v>
       </c>
@@ -17495,7 +17508,7 @@
         <v>30908.863333333331</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A283" s="95" t="s">
         <v>71</v>
       </c>
@@ -17509,7 +17522,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A284" s="98" t="s">
         <v>72</v>
       </c>
@@ -17523,7 +17536,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A285" s="98" t="s">
         <v>72</v>
       </c>
@@ -17537,7 +17550,7 @@
         <v>75702.7</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A286" s="98" t="s">
         <v>72</v>
       </c>
@@ -17551,7 +17564,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A287" s="98" t="s">
         <v>72</v>
       </c>
@@ -17565,7 +17578,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A288" s="98" t="s">
         <v>72</v>
       </c>
@@ -17579,7 +17592,7 @@
         <v>31157.318887999998</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A289" s="98" t="s">
         <v>72</v>
       </c>
@@ -17593,7 +17606,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A290" s="98" t="s">
         <v>72</v>
       </c>
@@ -17607,7 +17620,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A291" s="98" t="s">
         <v>72</v>
       </c>
@@ -17621,7 +17634,7 @@
         <v>5833.333333333333</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A292" s="95" t="s">
         <v>71</v>
       </c>
@@ -17635,7 +17648,7 @@
         <v>1407.0239328016664</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A293" s="95" t="s">
         <v>71</v>
       </c>
@@ -17649,7 +17662,7 @@
         <v>11666.666666666666</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A294" s="95" t="s">
         <v>71</v>
       </c>
@@ -17663,7 +17676,7 @@
         <v>865.16666666666674</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A295" s="95" t="s">
         <v>71</v>
       </c>
@@ -17677,7 +17690,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A296" s="95" t="s">
         <v>71</v>
       </c>
@@ -17691,7 +17704,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A297" s="95" t="s">
         <v>71</v>
       </c>
@@ -17705,7 +17718,7 @@
         <v>19749.776104941466</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A298" s="95" t="s">
         <v>71</v>
       </c>
@@ -17719,7 +17732,7 @@
         <v>19488.667569444446</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A299" s="95" t="s">
         <v>71</v>
       </c>
@@ -17733,7 +17746,7 @@
         <v>20833.333333333332</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A300" s="95" t="s">
         <v>71</v>
       </c>
@@ -17747,7 +17760,7 @@
         <v>1493.13924</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A301" s="95" t="s">
         <v>71</v>
       </c>
@@ -17761,7 +17774,7 @@
         <v>11277.666666666666</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A302" s="95" t="s">
         <v>71</v>
       </c>
@@ -17775,7 +17788,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A303" s="95" t="s">
         <v>71</v>
       </c>
@@ -17789,7 +17802,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A304" s="95" t="s">
         <v>71</v>
       </c>
@@ -17803,7 +17816,7 @@
         <v>337.06893333333335</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A305" s="95" t="s">
         <v>71</v>
       </c>
@@ -17817,7 +17830,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A306" s="95" t="s">
         <v>71</v>
       </c>
@@ -17831,7 +17844,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A307" s="95" t="s">
         <v>71</v>
       </c>
@@ -17845,7 +17858,7 @@
         <v>833.33333333333337</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A308" s="95" t="s">
         <v>71</v>
       </c>
@@ -17859,7 +17872,7 @@
         <v>614.26833333333332</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A309" s="95" t="s">
         <v>71</v>
       </c>
@@ -17873,7 +17886,7 @@
         <v>155.72999999999999</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A310" s="95" t="s">
         <v>71</v>
       </c>
@@ -17887,7 +17900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A311" s="95" t="s">
         <v>71</v>
       </c>
@@ -17901,7 +17914,7 @@
         <v>30908.863333333331</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A312" s="95" t="s">
         <v>71</v>
       </c>
@@ -17915,7 +17928,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A313" s="98" t="s">
         <v>72</v>
       </c>
@@ -17929,7 +17942,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A314" s="98" t="s">
         <v>72</v>
       </c>
@@ -17943,7 +17956,7 @@
         <v>75702.7</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A315" s="98" t="s">
         <v>72</v>
       </c>
@@ -17957,7 +17970,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A316" s="98" t="s">
         <v>72</v>
       </c>
@@ -17971,7 +17984,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A317" s="98" t="s">
         <v>72</v>
       </c>
@@ -17985,7 +17998,7 @@
         <v>31157.318887999998</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A318" s="98" t="s">
         <v>72</v>
       </c>
@@ -17999,7 +18012,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A319" s="98" t="s">
         <v>72</v>
       </c>
@@ -18013,7 +18026,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A320" s="98" t="s">
         <v>72</v>
       </c>
@@ -18027,7 +18040,7 @@
         <v>5833.333333333333</v>
       </c>
     </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A321" s="95" t="s">
         <v>71</v>
       </c>
@@ -18041,7 +18054,7 @@
         <v>1407.0239328016664</v>
       </c>
     </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A322" s="95" t="s">
         <v>71</v>
       </c>
@@ -18055,7 +18068,7 @@
         <v>11666.666666666666</v>
       </c>
     </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A323" s="95" t="s">
         <v>71</v>
       </c>
@@ -18069,7 +18082,7 @@
         <v>865.16666666666674</v>
       </c>
     </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A324" s="95" t="s">
         <v>71</v>
       </c>
@@ -18083,7 +18096,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A325" s="95" t="s">
         <v>71</v>
       </c>
@@ -18097,7 +18110,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A326" s="95" t="s">
         <v>71</v>
       </c>
@@ -18111,7 +18124,7 @@
         <v>19749.776104941466</v>
       </c>
     </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A327" s="95" t="s">
         <v>71</v>
       </c>
@@ -18125,7 +18138,7 @@
         <v>19488.667569444446</v>
       </c>
     </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A328" s="95" t="s">
         <v>71</v>
       </c>
@@ -18139,7 +18152,7 @@
         <v>20833.333333333332</v>
       </c>
     </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A329" s="95" t="s">
         <v>71</v>
       </c>
@@ -18153,7 +18166,7 @@
         <v>1493.13924</v>
       </c>
     </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A330" s="95" t="s">
         <v>71</v>
       </c>
@@ -18167,7 +18180,7 @@
         <v>11277.666666666666</v>
       </c>
     </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A331" s="95" t="s">
         <v>71</v>
       </c>
@@ -18181,7 +18194,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A332" s="95" t="s">
         <v>71</v>
       </c>
@@ -18195,7 +18208,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A333" s="95" t="s">
         <v>71</v>
       </c>
@@ -18209,7 +18222,7 @@
         <v>337.06893333333335</v>
       </c>
     </row>
-    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A334" s="95" t="s">
         <v>71</v>
       </c>
@@ -18223,7 +18236,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A335" s="95" t="s">
         <v>71</v>
       </c>
@@ -18237,7 +18250,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A336" s="95" t="s">
         <v>71</v>
       </c>
@@ -18251,7 +18264,7 @@
         <v>833.33333333333337</v>
       </c>
     </row>
-    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A337" s="95" t="s">
         <v>71</v>
       </c>
@@ -18265,7 +18278,7 @@
         <v>614.26833333333332</v>
       </c>
     </row>
-    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A338" s="95" t="s">
         <v>71</v>
       </c>
@@ -18279,7 +18292,7 @@
         <v>1483.5878</v>
       </c>
     </row>
-    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A339" s="95" t="s">
         <v>71</v>
       </c>
@@ -18293,7 +18306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A340" s="95" t="s">
         <v>71</v>
       </c>
@@ -18307,7 +18320,7 @@
         <v>30908.863333333331</v>
       </c>
     </row>
-    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A341" s="95" t="s">
         <v>71</v>
       </c>
@@ -18321,7 +18334,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A342" s="98" t="s">
         <v>72</v>
       </c>
@@ -18335,7 +18348,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A343" s="98" t="s">
         <v>72</v>
       </c>
@@ -18349,7 +18362,7 @@
         <v>75702.7</v>
       </c>
     </row>
-    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A344" s="98" t="s">
         <v>72</v>
       </c>
@@ -18363,7 +18376,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A345" s="98" t="s">
         <v>72</v>
       </c>
@@ -18377,7 +18390,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A346" s="98" t="s">
         <v>72</v>
       </c>
@@ -18391,7 +18404,7 @@
         <v>31157.318887999998</v>
       </c>
     </row>
-    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A347" s="98" t="s">
         <v>72</v>
       </c>
@@ -18405,7 +18418,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A348" s="98" t="s">
         <v>72</v>
       </c>
@@ -18419,7 +18432,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="349" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A349" s="98" t="s">
         <v>72</v>
       </c>

</xml_diff>

<commit_message>
cut rows and columns
</commit_message>
<xml_diff>
--- a/src/data/Acompanhamento Orçamento OPEX - Agosto2024 - Copia.xlsx
+++ b/src/data/Acompanhamento Orçamento OPEX - Agosto2024 - Copia.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anderson.bones\Desktop\Projetos\Python\opex-fs\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anderson\Desktop\OPEX\opex-fs\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C47B194-87FB-4210-8DC2-10A9FD645D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C54518-1E49-47C9-8C68-F3BE199D58D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="552" windowWidth="23016" windowHeight="11688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10065" yWindow="1845" windowWidth="26595" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meses" sheetId="1" r:id="rId1"/>
@@ -22,34 +22,21 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId4"/>
-    <pivotCache cacheId="10" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -64,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="80">
   <si>
     <t>Budget</t>
   </si>
@@ -325,21 +312,6 @@
   </si>
   <si>
     <t>Δ YTD Budget</t>
-  </si>
-  <si>
-    <t>budget</t>
-  </si>
-  <si>
-    <t>realizado</t>
-  </si>
-  <si>
-    <t>projetado</t>
-  </si>
-  <si>
-    <t>forecast</t>
-  </si>
-  <si>
-    <t>economia</t>
   </si>
 </sst>
 </file>
@@ -5792,7 +5764,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CABA5277-C369-4823-82A1-268B72B3CD5C}" name="Tabela dinâmica21" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="26" rowHeaderCaption="Despesa">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CABA5277-C369-4823-82A1-268B72B3CD5C}" name="Tabela dinâmica21" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="26" rowHeaderCaption="Despesa">
   <location ref="I6:L15" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -6252,6 +6224,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1">
         <x14:conditionalFormats count="2">
+          <x14:conditionalFormat priority="5" id="{57A22362-E8D4-43C1-8382-FF9EC3A2FC8B}">
+            <x14:pivotAreas count="1">
+              <pivotArea type="data" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+                <references count="1">
+                  <reference field="4294967294" count="1" selected="0">
+                    <x v="2"/>
+                  </reference>
+                </references>
+              </pivotArea>
+            </x14:pivotAreas>
+          </x14:conditionalFormat>
           <x14:conditionalFormat priority="6" id="{2F1A8382-0BB3-4B69-85C0-D1EEF9D80BA3}">
             <x14:pivotAreas count="1">
               <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
@@ -6273,17 +6256,6 @@
               </pivotArea>
             </x14:pivotAreas>
           </x14:conditionalFormat>
-          <x14:conditionalFormat priority="5" id="{57A22362-E8D4-43C1-8382-FF9EC3A2FC8B}">
-            <x14:pivotAreas count="1">
-              <pivotArea type="data" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-                <references count="1">
-                  <reference field="4294967294" count="1" selected="0">
-                    <x v="2"/>
-                  </reference>
-                </references>
-              </pivotArea>
-            </x14:pivotAreas>
-          </x14:conditionalFormat>
         </x14:conditionalFormats>
       </x14:pivotTableDefinition>
     </ext>
@@ -6295,7 +6267,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BB6324FA-1E30-400D-99B4-D79F50C7A0F6}" name="Tabela dinâmica1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BB6324FA-1E30-400D-99B4-D79F50C7A0F6}" name="Tabela dinâmica1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F2:S28" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -6855,31 +6827,31 @@
   <dimension ref="A4:AJ70"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="20.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.69921875" style="1" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="49.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="9.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.75" style="1" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="49.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="9.25" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.3984375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.375" style="1" customWidth="1"/>
     <col min="20" max="20" width="11" style="1" customWidth="1"/>
     <col min="21" max="21" width="41" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="20.69921875" style="1"/>
+    <col min="22" max="16384" width="20.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B4" s="116" t="s">
         <v>48</v>
       </c>
@@ -6921,7 +6893,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B5" s="117"/>
       <c r="C5" s="113"/>
       <c r="D5" s="113"/>
@@ -6967,7 +6939,7 @@
       <c r="T5" s="113"/>
       <c r="U5" s="115"/>
     </row>
-    <row r="6" spans="1:36" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -6981,7 +6953,7 @@
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>49</v>
       </c>
@@ -7065,7 +7037,7 @@
         <v>99813.228342604591</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B8"/>
       <c r="C8"/>
       <c r="D8"/>
@@ -7091,7 +7063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
         <v>5</v>
       </c>
@@ -7176,7 +7148,7 @@
       <c r="AI9" s="8"/>
       <c r="AJ9" s="8"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>40120101</v>
       </c>
@@ -7257,7 +7229,7 @@
       <c r="AI10" s="8"/>
       <c r="AJ10" s="8"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>40120102</v>
       </c>
@@ -7344,7 +7316,7 @@
       <c r="AI11" s="8"/>
       <c r="AJ11" s="8"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>40120103</v>
       </c>
@@ -7427,7 +7399,7 @@
       <c r="AI12" s="8"/>
       <c r="AJ12" s="8"/>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
         <v>9</v>
       </c>
@@ -7510,7 +7482,7 @@
       <c r="AI13" s="8"/>
       <c r="AJ13" s="8"/>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>40120201</v>
       </c>
@@ -7592,7 +7564,7 @@
       <c r="AI14" s="8"/>
       <c r="AJ14" s="8"/>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -7629,7 +7601,7 @@
       <c r="AI15" s="8"/>
       <c r="AJ15" s="8"/>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B16" s="13" t="s">
         <v>11</v>
       </c>
@@ -7711,7 +7683,7 @@
       <c r="AI16" s="8"/>
       <c r="AJ16" s="8"/>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>40120401</v>
       </c>
@@ -7795,7 +7767,7 @@
       <c r="AI17" s="8"/>
       <c r="AJ17" s="8"/>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>40120402</v>
       </c>
@@ -7879,7 +7851,7 @@
       <c r="AI18" s="8"/>
       <c r="AJ18" s="8"/>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>40120403</v>
       </c>
@@ -7963,7 +7935,7 @@
       <c r="AI19" s="8"/>
       <c r="AJ19" s="8"/>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>40120404</v>
       </c>
@@ -8047,7 +8019,7 @@
       <c r="AI20" s="8"/>
       <c r="AJ20" s="8"/>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
@@ -8084,7 +8056,7 @@
       <c r="AI21" s="8"/>
       <c r="AJ21" s="8"/>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B22" s="13" t="s">
         <v>16</v>
       </c>
@@ -8166,7 +8138,7 @@
       <c r="AI22" s="8"/>
       <c r="AJ22" s="8"/>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>40120501</v>
       </c>
@@ -8250,7 +8222,7 @@
       <c r="AI23" s="8"/>
       <c r="AJ23" s="8"/>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>40120503</v>
       </c>
@@ -8334,7 +8306,7 @@
       <c r="AI24" s="8"/>
       <c r="AJ24" s="8"/>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B25" s="13" t="s">
         <v>19</v>
       </c>
@@ -8416,7 +8388,7 @@
       <c r="AI25" s="8"/>
       <c r="AJ25" s="8"/>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>40120601</v>
       </c>
@@ -8490,7 +8462,7 @@
       <c r="AI26" s="8"/>
       <c r="AJ26" s="8"/>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>40120602</v>
       </c>
@@ -8574,7 +8546,7 @@
       <c r="AI27" s="8"/>
       <c r="AJ27" s="8"/>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>40120605</v>
       </c>
@@ -8646,7 +8618,7 @@
       <c r="AI28" s="8"/>
       <c r="AJ28" s="8"/>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>40120603</v>
       </c>
@@ -8708,7 +8680,7 @@
       <c r="AI29" s="8"/>
       <c r="AJ29" s="8"/>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>40120606</v>
       </c>
@@ -8786,7 +8758,7 @@
       <c r="AI30" s="8"/>
       <c r="AJ30" s="8"/>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>40120612</v>
       </c>
@@ -8870,7 +8842,7 @@
       <c r="AI31" s="8"/>
       <c r="AJ31" s="8"/>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>40120613</v>
       </c>
@@ -8946,7 +8918,7 @@
       <c r="AI32" s="8"/>
       <c r="AJ32" s="8"/>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>40120614</v>
       </c>
@@ -9026,7 +8998,7 @@
       <c r="AI33" s="8"/>
       <c r="AJ33" s="8"/>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B34" s="14"/>
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
@@ -9063,7 +9035,7 @@
       <c r="AI34" s="8"/>
       <c r="AJ34" s="8"/>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B35" s="13" t="s">
         <v>27</v>
       </c>
@@ -9145,7 +9117,7 @@
       <c r="AI35" s="8"/>
       <c r="AJ35" s="8"/>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>40120701</v>
       </c>
@@ -9227,7 +9199,7 @@
       <c r="AI36" s="8"/>
       <c r="AJ36" s="8"/>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>40120705</v>
       </c>
@@ -9309,7 +9281,7 @@
       <c r="AI37" s="8"/>
       <c r="AJ37" s="8"/>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>40120706</v>
       </c>
@@ -9387,7 +9359,7 @@
       <c r="AI38" s="8"/>
       <c r="AJ38" s="8"/>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>40120707</v>
       </c>
@@ -9463,7 +9435,7 @@
       <c r="AI39" s="8"/>
       <c r="AJ39" s="8"/>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B40" s="14"/>
       <c r="C40" s="17"/>
       <c r="D40" s="17"/>
@@ -9500,7 +9472,7 @@
       <c r="AI40" s="8"/>
       <c r="AJ40" s="8"/>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B41" s="13" t="s">
         <v>32</v>
       </c>
@@ -9574,7 +9546,7 @@
       <c r="AI41" s="8"/>
       <c r="AJ41" s="8"/>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40120801</v>
       </c>
@@ -9648,7 +9620,7 @@
       <c r="AI42" s="8"/>
       <c r="AJ42" s="8"/>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>40120804</v>
       </c>
@@ -9724,7 +9696,7 @@
       <c r="AI43" s="8"/>
       <c r="AJ43" s="8"/>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B44" s="14"/>
       <c r="C44" s="17"/>
       <c r="D44" s="17"/>
@@ -9761,7 +9733,7 @@
       <c r="AI44" s="8"/>
       <c r="AJ44" s="8"/>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B45" s="13" t="s">
         <v>35</v>
       </c>
@@ -9835,7 +9807,7 @@
       <c r="AI45" s="8"/>
       <c r="AJ45" s="8"/>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>40120901</v>
       </c>
@@ -9911,7 +9883,7 @@
       <c r="AI46" s="8"/>
       <c r="AJ46" s="8"/>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B47" s="14"/>
       <c r="C47" s="17"/>
       <c r="D47" s="17"/>
@@ -9948,7 +9920,7 @@
       <c r="AI47" s="8"/>
       <c r="AJ47" s="8"/>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B48" s="13" t="s">
         <v>37</v>
       </c>
@@ -10030,7 +10002,7 @@
       <c r="AI48" s="8"/>
       <c r="AJ48" s="8"/>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>40121102</v>
       </c>
@@ -10112,7 +10084,7 @@
       <c r="AI49" s="8"/>
       <c r="AJ49" s="8"/>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>40121104</v>
       </c>
@@ -10186,7 +10158,7 @@
       <c r="AI50" s="8"/>
       <c r="AJ50" s="8"/>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>40121107</v>
       </c>
@@ -10262,7 +10234,7 @@
       <c r="AI51" s="8"/>
       <c r="AJ51" s="8"/>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>40121108</v>
       </c>
@@ -10336,7 +10308,7 @@
       <c r="AI52" s="8"/>
       <c r="AJ52" s="8"/>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>40121110</v>
       </c>
@@ -10416,7 +10388,7 @@
       <c r="AI53" s="8"/>
       <c r="AJ53" s="8"/>
     </row>
-    <row r="54" spans="1:36" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:36" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>40121113</v>
       </c>
@@ -10498,7 +10470,7 @@
       <c r="AI54" s="8"/>
       <c r="AJ54" s="8"/>
     </row>
-    <row r="55" spans="1:36" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:36" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>40121119</v>
       </c>
@@ -10582,7 +10554,7 @@
       <c r="AI55" s="8"/>
       <c r="AJ55" s="8"/>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>40121120</v>
       </c>
@@ -10658,7 +10630,7 @@
       <c r="AI56" s="8"/>
       <c r="AJ56" s="8"/>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>40121122</v>
       </c>
@@ -10735,59 +10707,34 @@
       <c r="AI57" s="8"/>
       <c r="AJ57" s="8"/>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="D60" s="108" t="s">
-        <v>80</v>
-      </c>
-      <c r="E60" s="109">
-        <f>C7</f>
-        <v>4963678.32</v>
-      </c>
+    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="D60" s="108"/>
+      <c r="E60" s="109"/>
       <c r="H60" s="105"/>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="D61" s="108" t="s">
-        <v>81</v>
-      </c>
-      <c r="E61" s="110">
-        <f>SUM(E7:I7)</f>
-        <v>1964632.26</v>
-      </c>
-    </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="D62" s="108" t="s">
-        <v>82</v>
-      </c>
-      <c r="E62" s="110">
-        <f>SUM(J7:P7)</f>
-        <v>2859627.79</v>
-      </c>
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="D61" s="108"/>
+      <c r="E61" s="110"/>
+    </row>
+    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="D62" s="108"/>
+      <c r="E62" s="110"/>
       <c r="I62" s="105"/>
       <c r="O62" s="105"/>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="D63" s="108" t="s">
-        <v>83</v>
-      </c>
-      <c r="E63" s="111">
-        <f>E61+E62</f>
-        <v>4824260.05</v>
-      </c>
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="D63" s="108"/>
+      <c r="E63" s="111"/>
       <c r="H63" s="105"/>
       <c r="K63" s="105"/>
       <c r="M63" s="105"/>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="D64" s="108" t="s">
-        <v>84</v>
-      </c>
-      <c r="E64" s="110">
-        <f>E60-E63</f>
-        <v>139418.27000000048</v>
-      </c>
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="D64" s="108"/>
+      <c r="E64" s="110"/>
       <c r="H64" s="105"/>
     </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E70" s="106"/>
     </row>
   </sheetData>
@@ -10859,32 +10806,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D5B6C47-1CA6-4048-879D-E4787523BC8A}">
   <dimension ref="B1:N51"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D52" sqref="D47:F52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.09765625" customWidth="1"/>
+    <col min="1" max="1" width="2.125" customWidth="1"/>
     <col min="2" max="2" width="47" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="23.59765625" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="23.625" style="31" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" style="32" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="1.5" customWidth="1"/>
     <col min="9" max="9" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15.375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.59765625" customWidth="1"/>
-    <col min="15" max="20" width="6.8984375" bestFit="1" customWidth="1"/>
-    <col min="21" max="30" width="7.8984375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.8984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.625" customWidth="1"/>
+    <col min="15" max="20" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="21" max="30" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="120" t="s">
         <v>62</v>
       </c>
@@ -10901,7 +10848,7 @@
       <c r="M2" s="121"/>
       <c r="N2" s="51"/>
     </row>
-    <row r="3" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="122"/>
       <c r="C3" s="123"/>
       <c r="D3" s="123"/>
@@ -10916,11 +10863,11 @@
       <c r="M3" s="123"/>
       <c r="N3" s="69"/>
     </row>
-    <row r="4" spans="2:14" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="36"/>
       <c r="N4" s="37"/>
     </row>
-    <row r="5" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="68" t="s">
         <v>61</v>
       </c>
@@ -10929,7 +10876,7 @@
       </c>
       <c r="N5" s="37"/>
     </row>
-    <row r="6" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="38" t="s">
         <v>50</v>
       </c>
@@ -10965,7 +10912,7 @@
       </c>
       <c r="N6" s="37"/>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="43" t="s">
         <v>5</v>
       </c>
@@ -11006,7 +10953,7 @@
       </c>
       <c r="N7" s="37"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="43" t="s">
         <v>5</v>
       </c>
@@ -11047,7 +10994,7 @@
       </c>
       <c r="N8" s="37"/>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="43" t="s">
         <v>5</v>
       </c>
@@ -11087,7 +11034,7 @@
       </c>
       <c r="N9" s="37"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="43" t="s">
         <v>9</v>
       </c>
@@ -11128,7 +11075,7 @@
       </c>
       <c r="N10" s="37"/>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="43" t="s">
         <v>11</v>
       </c>
@@ -11169,7 +11116,7 @@
       </c>
       <c r="N11" s="37"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="43" t="s">
         <v>11</v>
       </c>
@@ -11210,7 +11157,7 @@
       </c>
       <c r="N12" s="37"/>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="43" t="s">
         <v>11</v>
       </c>
@@ -11251,7 +11198,7 @@
       </c>
       <c r="N13" s="37"/>
     </row>
-    <row r="14" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="43" t="s">
         <v>11</v>
       </c>
@@ -11292,7 +11239,7 @@
       </c>
       <c r="N14" s="37"/>
     </row>
-    <row r="15" spans="2:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:14" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="43" t="s">
         <v>16</v>
       </c>
@@ -11333,7 +11280,7 @@
       </c>
       <c r="N15" s="52"/>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="43" t="s">
         <v>16</v>
       </c>
@@ -11358,7 +11305,7 @@
       </c>
       <c r="N16" s="37"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="43" t="s">
         <v>19</v>
       </c>
@@ -11386,7 +11333,7 @@
       </c>
       <c r="N17" s="37"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="43" t="s">
         <v>19</v>
       </c>
@@ -11418,7 +11365,7 @@
       <c r="M18" s="119"/>
       <c r="N18" s="37"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="43" t="s">
         <v>19</v>
       </c>
@@ -11448,7 +11395,7 @@
       <c r="M19" s="72"/>
       <c r="N19" s="37"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="43" t="s">
         <v>19</v>
       </c>
@@ -11488,7 +11435,7 @@
       </c>
       <c r="N20" s="37"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="43" t="s">
         <v>19</v>
       </c>
@@ -11532,7 +11479,7 @@
       </c>
       <c r="N21" s="37"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="43" t="s">
         <v>19</v>
       </c>
@@ -11576,7 +11523,7 @@
       </c>
       <c r="N22" s="37"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="43" t="s">
         <v>19</v>
       </c>
@@ -11620,7 +11567,7 @@
       </c>
       <c r="N23" s="37"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="43" t="s">
         <v>19</v>
       </c>
@@ -11664,7 +11611,7 @@
       </c>
       <c r="N24" s="37"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="43" t="s">
         <v>27</v>
       </c>
@@ -11708,7 +11655,7 @@
       </c>
       <c r="N25" s="37"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="43" t="s">
         <v>27</v>
       </c>
@@ -11752,7 +11699,7 @@
       </c>
       <c r="N26" s="37"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="43" t="s">
         <v>27</v>
       </c>
@@ -11796,7 +11743,7 @@
       </c>
       <c r="N27" s="37"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="43" t="s">
         <v>27</v>
       </c>
@@ -11840,7 +11787,7 @@
       </c>
       <c r="N28" s="37"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="43" t="s">
         <v>27</v>
       </c>
@@ -11884,7 +11831,7 @@
       </c>
       <c r="N29" s="37"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="43" t="s">
         <v>27</v>
       </c>
@@ -11909,7 +11856,7 @@
       </c>
       <c r="N30" s="37"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="43" t="s">
         <v>35</v>
       </c>
@@ -11934,7 +11881,7 @@
       </c>
       <c r="N31" s="53"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="43" t="s">
         <v>37</v>
       </c>
@@ -11959,7 +11906,7 @@
       </c>
       <c r="N32" s="37"/>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="43" t="s">
         <v>37</v>
       </c>
@@ -11984,7 +11931,7 @@
       </c>
       <c r="N33" s="37"/>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="43" t="s">
         <v>37</v>
       </c>
@@ -12016,7 +11963,7 @@
       <c r="M34" s="128"/>
       <c r="N34" s="37"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="43" t="s">
         <v>37</v>
       </c>
@@ -12046,7 +11993,7 @@
       <c r="M35" s="131"/>
       <c r="N35" s="37"/>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="43" t="s">
         <v>37</v>
       </c>
@@ -12076,7 +12023,7 @@
       <c r="M36" s="131"/>
       <c r="N36" s="37"/>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" s="43" t="s">
         <v>37</v>
       </c>
@@ -12106,7 +12053,7 @@
       <c r="M37" s="131"/>
       <c r="N37" s="37"/>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" s="43" t="s">
         <v>37</v>
       </c>
@@ -12136,7 +12083,7 @@
       <c r="M38" s="131"/>
       <c r="N38" s="37"/>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" s="43" t="s">
         <v>37</v>
       </c>
@@ -12166,7 +12113,7 @@
       <c r="M39" s="131"/>
       <c r="N39" s="37"/>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B40" s="59" t="s">
         <v>37</v>
       </c>
@@ -12196,7 +12143,7 @@
       <c r="M40" s="131"/>
       <c r="N40" s="70"/>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B41" s="124" t="s">
         <v>47</v>
       </c>
@@ -12225,7 +12172,7 @@
       <c r="M41" s="134"/>
       <c r="N41" s="70"/>
     </row>
-    <row r="42" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="55"/>
       <c r="C42" s="44"/>
       <c r="D42" s="56"/>
@@ -12240,13 +12187,13 @@
       <c r="M42" s="44"/>
       <c r="N42" s="54"/>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D48" s="107"/>
     </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E49" s="107"/>
     </row>
-    <row r="51" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D51" s="107"/>
     </row>
   </sheetData>
@@ -12333,37 +12280,37 @@
       <selection activeCell="G4" sqref="G4:K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.8984375" customWidth="1"/>
-    <col min="4" max="5" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.875" customWidth="1"/>
+    <col min="4" max="5" width="11.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.8984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="18" width="13.8984375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.09765625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.19921875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.09765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="18" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.3984375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.19921875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.19921875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.25" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="8" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.09765625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="8" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.69921875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.8984375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="93" t="s">
         <v>70</v>
       </c>
@@ -12377,7 +12324,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="95" t="s">
         <v>71</v>
       </c>
@@ -12397,7 +12344,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="95" t="s">
         <v>71</v>
       </c>
@@ -12456,7 +12403,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="95" t="s">
         <v>71</v>
       </c>
@@ -12516,7 +12463,7 @@
         <v>7035.1196640083326</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="95" t="s">
         <v>71</v>
       </c>
@@ -12576,7 +12523,7 @@
         <v>58333.333333333328</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="95" t="s">
         <v>71</v>
       </c>
@@ -12636,7 +12583,7 @@
         <v>4325.8333333333339</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="95" t="s">
         <v>71</v>
       </c>
@@ -12696,7 +12643,7 @@
         <v>115000</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="95" t="s">
         <v>71</v>
       </c>
@@ -12756,7 +12703,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="95" t="s">
         <v>71</v>
       </c>
@@ -12816,7 +12763,7 @@
         <v>98748.880524707332</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="95" t="s">
         <v>71</v>
       </c>
@@ -12876,7 +12823,7 @@
         <v>97443.337847222225</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="95" t="s">
         <v>71</v>
       </c>
@@ -12936,7 +12883,7 @@
         <v>104166.66666666666</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="95" t="s">
         <v>71</v>
       </c>
@@ -12996,7 +12943,7 @@
         <v>7465.6962000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="95" t="s">
         <v>71</v>
       </c>
@@ -13056,7 +13003,7 @@
         <v>41666.666666666672</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="95" t="s">
         <v>71</v>
       </c>
@@ -13116,7 +13063,7 @@
         <v>434901.83333333337</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="95" t="s">
         <v>71</v>
       </c>
@@ -13176,7 +13123,7 @@
         <v>83333.333333333343</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="95" t="s">
         <v>71</v>
       </c>
@@ -13236,7 +13183,7 @@
         <v>41666.666666666672</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="95" t="s">
         <v>71</v>
       </c>
@@ -13296,7 +13243,7 @@
         <v>1685.3446666666669</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="95" t="s">
         <v>71</v>
       </c>
@@ -13356,7 +13303,7 @@
         <v>8651.6666666666679</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="95" t="s">
         <v>71</v>
       </c>
@@ -13416,7 +13363,7 @@
         <v>166666.66666666669</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="95" t="s">
         <v>71</v>
       </c>
@@ -13476,7 +13423,7 @@
         <v>8651.6666666666679</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="95" t="s">
         <v>71</v>
       </c>
@@ -13536,7 +13483,7 @@
         <v>4166.666666666667</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="95" t="s">
         <v>71</v>
       </c>
@@ -13596,7 +13543,7 @@
         <v>3071.3416666666667</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="98" t="s">
         <v>72</v>
       </c>
@@ -13656,7 +13603,7 @@
         <v>467.18999999999994</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="98" t="s">
         <v>72</v>
       </c>
@@ -13716,7 +13663,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="98" t="s">
         <v>72</v>
       </c>
@@ -13776,7 +13723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="98" t="s">
         <v>72</v>
       </c>
@@ -13836,7 +13783,7 @@
         <v>310330.91110666667</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="98" t="s">
         <v>72</v>
       </c>
@@ -13896,7 +13843,7 @@
         <v>41666.666666666657</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="98" t="s">
         <v>72</v>
       </c>
@@ -13952,7 +13899,7 @@
         <v>4963678.6716222521</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="98" t="s">
         <v>72</v>
       </c>
@@ -13966,7 +13913,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="98" t="s">
         <v>72</v>
       </c>
@@ -13980,7 +13927,7 @@
         <v>5833.333333333333</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="95" t="s">
         <v>71</v>
       </c>
@@ -13994,7 +13941,7 @@
         <v>1407.0239328016664</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="95" t="s">
         <v>71</v>
       </c>
@@ -14008,7 +13955,7 @@
         <v>11666.666666666666</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="95" t="s">
         <v>71</v>
       </c>
@@ -14022,7 +13969,7 @@
         <v>865.16666666666674</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="95" t="s">
         <v>71</v>
       </c>
@@ -14036,7 +13983,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="95" t="s">
         <v>71</v>
       </c>
@@ -14050,7 +13997,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="95" t="s">
         <v>71</v>
       </c>
@@ -14064,7 +14011,7 @@
         <v>19749.776104941466</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="95" t="s">
         <v>71</v>
       </c>
@@ -14078,7 +14025,7 @@
         <v>19488.667569444446</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="95" t="s">
         <v>71</v>
       </c>
@@ -14092,7 +14039,7 @@
         <v>20833.333333333332</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="95" t="s">
         <v>71</v>
       </c>
@@ -14106,7 +14053,7 @@
         <v>1493.13924</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="95" t="s">
         <v>71</v>
       </c>
@@ -14120,7 +14067,7 @@
         <v>11277.666666666666</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="95" t="s">
         <v>71</v>
       </c>
@@ -14134,7 +14081,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="95" t="s">
         <v>71</v>
       </c>
@@ -14148,7 +14095,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="95" t="s">
         <v>71</v>
       </c>
@@ -14162,7 +14109,7 @@
         <v>337.06893333333335</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="95" t="s">
         <v>71</v>
       </c>
@@ -14176,7 +14123,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="95" t="s">
         <v>71</v>
       </c>
@@ -14190,7 +14137,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="95" t="s">
         <v>71</v>
       </c>
@@ -14204,7 +14151,7 @@
         <v>833.33333333333337</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="95" t="s">
         <v>71</v>
       </c>
@@ -14218,7 +14165,7 @@
         <v>614.26833333333332</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="95" t="s">
         <v>71</v>
       </c>
@@ -14232,7 +14179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="95" t="s">
         <v>71</v>
       </c>
@@ -14246,7 +14193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="95" t="s">
         <v>71</v>
       </c>
@@ -14260,7 +14207,7 @@
         <v>30908.863333333331</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="95" t="s">
         <v>71</v>
       </c>
@@ -14274,7 +14221,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="98" t="s">
         <v>72</v>
       </c>
@@ -14288,7 +14235,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="98" t="s">
         <v>72</v>
       </c>
@@ -14302,7 +14249,7 @@
         <v>75702.7</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="98" t="s">
         <v>72</v>
       </c>
@@ -14316,7 +14263,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="98" t="s">
         <v>72</v>
       </c>
@@ -14330,7 +14277,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="98" t="s">
         <v>72</v>
       </c>
@@ -14344,7 +14291,7 @@
         <v>31157.318887999998</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="98" t="s">
         <v>72</v>
       </c>
@@ -14358,7 +14305,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="98" t="s">
         <v>72</v>
       </c>
@@ -14372,7 +14319,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="98" t="s">
         <v>72</v>
       </c>
@@ -14386,7 +14333,7 @@
         <v>5833.333333333333</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="95" t="s">
         <v>71</v>
       </c>
@@ -14400,7 +14347,7 @@
         <v>1407.0239328016664</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="95" t="s">
         <v>71</v>
       </c>
@@ -14414,7 +14361,7 @@
         <v>11666.666666666666</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="95" t="s">
         <v>71</v>
       </c>
@@ -14428,7 +14375,7 @@
         <v>865.16666666666674</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="95" t="s">
         <v>71</v>
       </c>
@@ -14442,7 +14389,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="95" t="s">
         <v>71</v>
       </c>
@@ -14456,7 +14403,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="95" t="s">
         <v>71</v>
       </c>
@@ -14470,7 +14417,7 @@
         <v>19749.776104941466</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="95" t="s">
         <v>71</v>
       </c>
@@ -14484,7 +14431,7 @@
         <v>19488.667569444446</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="95" t="s">
         <v>71</v>
       </c>
@@ -14498,7 +14445,7 @@
         <v>20833.333333333332</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="95" t="s">
         <v>71</v>
       </c>
@@ -14512,7 +14459,7 @@
         <v>1493.13924</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="95" t="s">
         <v>71</v>
       </c>
@@ -14526,7 +14473,7 @@
         <v>11277.666666666666</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="95" t="s">
         <v>71</v>
       </c>
@@ -14540,7 +14487,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="95" t="s">
         <v>71</v>
       </c>
@@ -14554,7 +14501,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="95" t="s">
         <v>71</v>
       </c>
@@ -14568,7 +14515,7 @@
         <v>337.06893333333335</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="95" t="s">
         <v>71</v>
       </c>
@@ -14582,7 +14529,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="95" t="s">
         <v>71</v>
       </c>
@@ -14596,7 +14543,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="95" t="s">
         <v>71</v>
       </c>
@@ -14610,7 +14557,7 @@
         <v>833.33333333333337</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="95" t="s">
         <v>71</v>
       </c>
@@ -14624,7 +14571,7 @@
         <v>614.26833333333332</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="95" t="s">
         <v>71</v>
       </c>
@@ -14638,7 +14585,7 @@
         <v>155.72999999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="95" t="s">
         <v>71</v>
       </c>
@@ -14652,7 +14599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="95" t="s">
         <v>71</v>
       </c>
@@ -14666,7 +14613,7 @@
         <v>30908.863333333331</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="95" t="s">
         <v>71</v>
       </c>
@@ -14680,7 +14627,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="98" t="s">
         <v>72</v>
       </c>
@@ -14694,7 +14641,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="98" t="s">
         <v>72</v>
       </c>
@@ -14708,7 +14655,7 @@
         <v>75702.7</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="98" t="s">
         <v>72</v>
       </c>
@@ -14722,7 +14669,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="98" t="s">
         <v>72</v>
       </c>
@@ -14736,7 +14683,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="98" t="s">
         <v>72</v>
       </c>
@@ -14750,7 +14697,7 @@
         <v>31157.318887999998</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="98" t="s">
         <v>72</v>
       </c>
@@ -14764,7 +14711,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="98" t="s">
         <v>72</v>
       </c>
@@ -14778,7 +14725,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="98" t="s">
         <v>72</v>
       </c>
@@ -14792,7 +14739,7 @@
         <v>5833.333333333333</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="95" t="s">
         <v>71</v>
       </c>
@@ -14806,7 +14753,7 @@
         <v>1407.0239328016664</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="95" t="s">
         <v>71</v>
       </c>
@@ -14820,7 +14767,7 @@
         <v>11666.666666666666</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="95" t="s">
         <v>71</v>
       </c>
@@ -14834,7 +14781,7 @@
         <v>865.16666666666674</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="95" t="s">
         <v>71</v>
       </c>
@@ -14848,7 +14795,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="95" t="s">
         <v>71</v>
       </c>
@@ -14862,7 +14809,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="95" t="s">
         <v>71</v>
       </c>
@@ -14876,7 +14823,7 @@
         <v>19749.776104941466</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="95" t="s">
         <v>71</v>
       </c>
@@ -14890,7 +14837,7 @@
         <v>19488.667569444446</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="95" t="s">
         <v>71</v>
       </c>
@@ -14904,7 +14851,7 @@
         <v>20833.333333333332</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="95" t="s">
         <v>71</v>
       </c>
@@ -14918,7 +14865,7 @@
         <v>1493.13924</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="95" t="s">
         <v>71</v>
       </c>
@@ -14932,7 +14879,7 @@
         <v>11277.666666666666</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="95" t="s">
         <v>71</v>
       </c>
@@ -14946,7 +14893,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="95" t="s">
         <v>71</v>
       </c>
@@ -14960,7 +14907,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="95" t="s">
         <v>71</v>
       </c>
@@ -14974,7 +14921,7 @@
         <v>337.06893333333335</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="95" t="s">
         <v>71</v>
       </c>
@@ -14988,7 +14935,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="95" t="s">
         <v>71</v>
       </c>
@@ -15002,7 +14949,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="95" t="s">
         <v>71</v>
       </c>
@@ -15016,7 +14963,7 @@
         <v>833.33333333333337</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="95" t="s">
         <v>71</v>
       </c>
@@ -15030,7 +14977,7 @@
         <v>614.26833333333332</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="95" t="s">
         <v>71</v>
       </c>
@@ -15044,7 +14991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="95" t="s">
         <v>71</v>
       </c>
@@ -15058,7 +15005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="95" t="s">
         <v>71</v>
       </c>
@@ -15072,7 +15019,7 @@
         <v>30908.863333333331</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="95" t="s">
         <v>71</v>
       </c>
@@ -15086,7 +15033,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="98" t="s">
         <v>72</v>
       </c>
@@ -15100,7 +15047,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="98" t="s">
         <v>72</v>
       </c>
@@ -15114,7 +15061,7 @@
         <v>75702.7</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="98" t="s">
         <v>72</v>
       </c>
@@ -15128,7 +15075,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="98" t="s">
         <v>72</v>
       </c>
@@ -15142,7 +15089,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="98" t="s">
         <v>72</v>
       </c>
@@ -15156,7 +15103,7 @@
         <v>31157.318887999998</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="98" t="s">
         <v>72</v>
       </c>
@@ -15170,7 +15117,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="98" t="s">
         <v>72</v>
       </c>
@@ -15184,7 +15131,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="98" t="s">
         <v>72</v>
       </c>
@@ -15198,7 +15145,7 @@
         <v>5833.333333333333</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="95" t="s">
         <v>71</v>
       </c>
@@ -15212,7 +15159,7 @@
         <v>1407.0239328016664</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="95" t="s">
         <v>71</v>
       </c>
@@ -15226,7 +15173,7 @@
         <v>11666.666666666666</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="95" t="s">
         <v>71</v>
       </c>
@@ -15240,7 +15187,7 @@
         <v>865.16666666666674</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="95" t="s">
         <v>71</v>
       </c>
@@ -15254,7 +15201,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="95" t="s">
         <v>71</v>
       </c>
@@ -15268,7 +15215,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="95" t="s">
         <v>71</v>
       </c>
@@ -15282,7 +15229,7 @@
         <v>19749.776104941466</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="95" t="s">
         <v>71</v>
       </c>
@@ -15296,7 +15243,7 @@
         <v>19488.667569444446</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="95" t="s">
         <v>71</v>
       </c>
@@ -15310,7 +15257,7 @@
         <v>20833.333333333332</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="95" t="s">
         <v>71</v>
       </c>
@@ -15324,7 +15271,7 @@
         <v>1493.13924</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="95" t="s">
         <v>71</v>
       </c>
@@ -15338,7 +15285,7 @@
         <v>11277.666666666666</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="95" t="s">
         <v>71</v>
       </c>
@@ -15352,7 +15299,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="95" t="s">
         <v>71</v>
       </c>
@@ -15366,7 +15313,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="95" t="s">
         <v>71</v>
       </c>
@@ -15380,7 +15327,7 @@
         <v>337.06893333333335</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="95" t="s">
         <v>71</v>
       </c>
@@ -15394,7 +15341,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="95" t="s">
         <v>71</v>
       </c>
@@ -15408,7 +15355,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="95" t="s">
         <v>71</v>
       </c>
@@ -15422,7 +15369,7 @@
         <v>833.33333333333337</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="95" t="s">
         <v>71</v>
       </c>
@@ -15436,7 +15383,7 @@
         <v>614.26833333333332</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="95" t="s">
         <v>71</v>
       </c>
@@ -15450,7 +15397,7 @@
         <v>155.72999999999999</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="95" t="s">
         <v>71</v>
       </c>
@@ -15464,7 +15411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="95" t="s">
         <v>71</v>
       </c>
@@ -15478,7 +15425,7 @@
         <v>30908.863333333331</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="95" t="s">
         <v>71</v>
       </c>
@@ -15492,7 +15439,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="98" t="s">
         <v>72</v>
       </c>
@@ -15506,7 +15453,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="98" t="s">
         <v>72</v>
       </c>
@@ -15520,7 +15467,7 @@
         <v>75702.7</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="98" t="s">
         <v>72</v>
       </c>
@@ -15534,7 +15481,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="98" t="s">
         <v>72</v>
       </c>
@@ -15548,7 +15495,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="98" t="s">
         <v>72</v>
       </c>
@@ -15562,7 +15509,7 @@
         <v>31157.318887999998</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="98" t="s">
         <v>72</v>
       </c>
@@ -15576,7 +15523,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="98" t="s">
         <v>72</v>
       </c>
@@ -15590,7 +15537,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="98" t="s">
         <v>72</v>
       </c>
@@ -15604,7 +15551,7 @@
         <v>5833.333333333333</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="95" t="s">
         <v>71</v>
       </c>
@@ -15618,7 +15565,7 @@
         <v>1407.0239328016664</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="95" t="s">
         <v>71</v>
       </c>
@@ -15632,7 +15579,7 @@
         <v>11666.666666666666</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="95" t="s">
         <v>71</v>
       </c>
@@ -15646,7 +15593,7 @@
         <v>865.16666666666674</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="95" t="s">
         <v>71</v>
       </c>
@@ -15660,7 +15607,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="95" t="s">
         <v>71</v>
       </c>
@@ -15674,7 +15621,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="95" t="s">
         <v>71</v>
       </c>
@@ -15688,7 +15635,7 @@
         <v>19749.776104941466</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="95" t="s">
         <v>71</v>
       </c>
@@ -15702,7 +15649,7 @@
         <v>19488.667569444446</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="95" t="s">
         <v>71</v>
       </c>
@@ -15716,7 +15663,7 @@
         <v>20833.333333333332</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="95" t="s">
         <v>71</v>
       </c>
@@ -15730,7 +15677,7 @@
         <v>1493.13924</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="95" t="s">
         <v>71</v>
       </c>
@@ -15744,7 +15691,7 @@
         <v>11277.666666666666</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="95" t="s">
         <v>71</v>
       </c>
@@ -15758,7 +15705,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="95" t="s">
         <v>71</v>
       </c>
@@ -15772,7 +15719,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="95" t="s">
         <v>71</v>
       </c>
@@ -15786,7 +15733,7 @@
         <v>337.06893333333335</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="95" t="s">
         <v>71</v>
       </c>
@@ -15800,7 +15747,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="95" t="s">
         <v>71</v>
       </c>
@@ -15814,7 +15761,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="95" t="s">
         <v>71</v>
       </c>
@@ -15828,7 +15775,7 @@
         <v>833.33333333333337</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="95" t="s">
         <v>71</v>
       </c>
@@ -15842,7 +15789,7 @@
         <v>614.26833333333332</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="95" t="s">
         <v>71</v>
       </c>
@@ -15856,7 +15803,7 @@
         <v>1483.5878</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="95" t="s">
         <v>71</v>
       </c>
@@ -15870,7 +15817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="95" t="s">
         <v>71</v>
       </c>
@@ -15884,7 +15831,7 @@
         <v>30908.863333333331</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="95" t="s">
         <v>71</v>
       </c>
@@ -15898,7 +15845,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="98" t="s">
         <v>72</v>
       </c>
@@ -15912,7 +15859,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="98" t="s">
         <v>72</v>
       </c>
@@ -15926,7 +15873,7 @@
         <v>75702.7</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="98" t="s">
         <v>72</v>
       </c>
@@ -15940,7 +15887,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="98" t="s">
         <v>72</v>
       </c>
@@ -15954,7 +15901,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="98" t="s">
         <v>72</v>
       </c>
@@ -15968,7 +15915,7 @@
         <v>31157.318887999998</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="98" t="s">
         <v>72</v>
       </c>
@@ -15982,7 +15929,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="98" t="s">
         <v>72</v>
       </c>
@@ -15996,7 +15943,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="98" t="s">
         <v>72</v>
       </c>
@@ -16010,7 +15957,7 @@
         <v>5833.333333333333</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="95" t="s">
         <v>71</v>
       </c>
@@ -16024,7 +15971,7 @@
         <v>1407.0239328016664</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="95" t="s">
         <v>71</v>
       </c>
@@ -16038,7 +15985,7 @@
         <v>11666.666666666666</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="95" t="s">
         <v>71</v>
       </c>
@@ -16052,7 +15999,7 @@
         <v>865.16666666666674</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="95" t="s">
         <v>71</v>
       </c>
@@ -16066,7 +16013,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="95" t="s">
         <v>71</v>
       </c>
@@ -16080,7 +16027,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="95" t="s">
         <v>71</v>
       </c>
@@ -16094,7 +16041,7 @@
         <v>19749.776104941466</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="95" t="s">
         <v>71</v>
       </c>
@@ -16108,7 +16055,7 @@
         <v>19488.667569444446</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="95" t="s">
         <v>71</v>
       </c>
@@ -16122,7 +16069,7 @@
         <v>20833.333333333332</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="95" t="s">
         <v>71</v>
       </c>
@@ -16136,7 +16083,7 @@
         <v>1493.13924</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="95" t="s">
         <v>71</v>
       </c>
@@ -16150,7 +16097,7 @@
         <v>11277.666666666666</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="95" t="s">
         <v>71</v>
       </c>
@@ -16164,7 +16111,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="95" t="s">
         <v>71</v>
       </c>
@@ -16178,7 +16125,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="95" t="s">
         <v>71</v>
       </c>
@@ -16192,7 +16139,7 @@
         <v>337.06893333333335</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="95" t="s">
         <v>71</v>
       </c>
@@ -16206,7 +16153,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="95" t="s">
         <v>71</v>
       </c>
@@ -16220,7 +16167,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="95" t="s">
         <v>71</v>
       </c>
@@ -16234,7 +16181,7 @@
         <v>833.33333333333337</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="95" t="s">
         <v>71</v>
       </c>
@@ -16248,7 +16195,7 @@
         <v>614.26833333333332</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="95" t="s">
         <v>71</v>
       </c>
@@ -16262,7 +16209,7 @@
         <v>155.72999999999999</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="95" t="s">
         <v>71</v>
       </c>
@@ -16276,7 +16223,7 @@
         <v>6229.2</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="95" t="s">
         <v>71</v>
       </c>
@@ -16290,7 +16237,7 @@
         <v>30908.863333333331</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="95" t="s">
         <v>71</v>
       </c>
@@ -16304,7 +16251,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="98" t="s">
         <v>72</v>
       </c>
@@ -16318,7 +16265,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="98" t="s">
         <v>72</v>
       </c>
@@ -16332,7 +16279,7 @@
         <v>75702.7</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="98" t="s">
         <v>72</v>
       </c>
@@ -16346,7 +16293,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="98" t="s">
         <v>72</v>
       </c>
@@ -16360,7 +16307,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="98" t="s">
         <v>72</v>
       </c>
@@ -16374,7 +16321,7 @@
         <v>31157.318887999998</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="98" t="s">
         <v>72</v>
       </c>
@@ -16388,7 +16335,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="98" t="s">
         <v>72</v>
       </c>
@@ -16402,7 +16349,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="98" t="s">
         <v>72</v>
       </c>
@@ -16416,7 +16363,7 @@
         <v>5833.333333333333</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="95" t="s">
         <v>71</v>
       </c>
@@ -16430,7 +16377,7 @@
         <v>1407.0239328016664</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="95" t="s">
         <v>71</v>
       </c>
@@ -16444,7 +16391,7 @@
         <v>11666.666666666666</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="95" t="s">
         <v>71</v>
       </c>
@@ -16458,7 +16405,7 @@
         <v>865.16666666666674</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="95" t="s">
         <v>71</v>
       </c>
@@ -16472,7 +16419,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="95" t="s">
         <v>71</v>
       </c>
@@ -16486,7 +16433,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="95" t="s">
         <v>71</v>
       </c>
@@ -16500,7 +16447,7 @@
         <v>19749.776104941466</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="95" t="s">
         <v>71</v>
       </c>
@@ -16514,7 +16461,7 @@
         <v>19488.667569444446</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="95" t="s">
         <v>71</v>
       </c>
@@ -16528,7 +16475,7 @@
         <v>20833.333333333332</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="95" t="s">
         <v>71</v>
       </c>
@@ -16542,7 +16489,7 @@
         <v>1493.13924</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="95" t="s">
         <v>71</v>
       </c>
@@ -16556,7 +16503,7 @@
         <v>11277.666666666666</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="95" t="s">
         <v>71</v>
       </c>
@@ -16570,7 +16517,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="95" t="s">
         <v>71</v>
       </c>
@@ -16584,7 +16531,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="95" t="s">
         <v>71</v>
       </c>
@@ -16598,7 +16545,7 @@
         <v>337.06893333333335</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="95" t="s">
         <v>71</v>
       </c>
@@ -16612,7 +16559,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="95" t="s">
         <v>71</v>
       </c>
@@ -16626,7 +16573,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="95" t="s">
         <v>71</v>
       </c>
@@ -16640,7 +16587,7 @@
         <v>833.33333333333337</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="95" t="s">
         <v>71</v>
       </c>
@@ -16654,7 +16601,7 @@
         <v>614.26833333333332</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="95" t="s">
         <v>71</v>
       </c>
@@ -16668,7 +16615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="95" t="s">
         <v>71</v>
       </c>
@@ -16682,7 +16629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="95" t="s">
         <v>71</v>
       </c>
@@ -16696,7 +16643,7 @@
         <v>30908.863333333331</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="95" t="s">
         <v>71</v>
       </c>
@@ -16710,7 +16657,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="98" t="s">
         <v>72</v>
       </c>
@@ -16724,7 +16671,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="98" t="s">
         <v>72</v>
       </c>
@@ -16738,7 +16685,7 @@
         <v>75702.7</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="98" t="s">
         <v>72</v>
       </c>
@@ -16752,7 +16699,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" s="98" t="s">
         <v>72</v>
       </c>
@@ -16766,7 +16713,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" s="98" t="s">
         <v>72</v>
       </c>
@@ -16780,7 +16727,7 @@
         <v>31157.318887999998</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" s="98" t="s">
         <v>72</v>
       </c>
@@ -16794,7 +16741,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" s="98" t="s">
         <v>72</v>
       </c>
@@ -16808,7 +16755,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" s="98" t="s">
         <v>72</v>
       </c>
@@ -16822,7 +16769,7 @@
         <v>5833.333333333333</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" s="95" t="s">
         <v>71</v>
       </c>
@@ -16836,7 +16783,7 @@
         <v>1407.0239328016664</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" s="95" t="s">
         <v>71</v>
       </c>
@@ -16850,7 +16797,7 @@
         <v>11666.666666666666</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" s="95" t="s">
         <v>71</v>
       </c>
@@ -16864,7 +16811,7 @@
         <v>865.16666666666674</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" s="95" t="s">
         <v>71</v>
       </c>
@@ -16878,7 +16825,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" s="95" t="s">
         <v>71</v>
       </c>
@@ -16892,7 +16839,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" s="95" t="s">
         <v>71</v>
       </c>
@@ -16906,7 +16853,7 @@
         <v>19749.776104941466</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" s="95" t="s">
         <v>71</v>
       </c>
@@ -16920,7 +16867,7 @@
         <v>19488.667569444446</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" s="95" t="s">
         <v>71</v>
       </c>
@@ -16934,7 +16881,7 @@
         <v>20833.333333333332</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" s="95" t="s">
         <v>71</v>
       </c>
@@ -16948,7 +16895,7 @@
         <v>1493.13924</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" s="95" t="s">
         <v>71</v>
       </c>
@@ -16962,7 +16909,7 @@
         <v>11277.666666666666</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" s="95" t="s">
         <v>71</v>
       </c>
@@ -16976,7 +16923,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" s="95" t="s">
         <v>71</v>
       </c>
@@ -16990,7 +16937,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" s="95" t="s">
         <v>71</v>
       </c>
@@ -17004,7 +16951,7 @@
         <v>337.06893333333335</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" s="95" t="s">
         <v>71</v>
       </c>
@@ -17018,7 +16965,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" s="95" t="s">
         <v>71</v>
       </c>
@@ -17032,7 +16979,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" s="95" t="s">
         <v>71</v>
       </c>
@@ -17046,7 +16993,7 @@
         <v>833.33333333333337</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" s="95" t="s">
         <v>71</v>
       </c>
@@ -17060,7 +17007,7 @@
         <v>614.26833333333332</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" s="95" t="s">
         <v>71</v>
       </c>
@@ -17074,7 +17021,7 @@
         <v>155.72999999999999</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" s="95" t="s">
         <v>71</v>
       </c>
@@ -17088,7 +17035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" s="95" t="s">
         <v>71</v>
       </c>
@@ -17102,7 +17049,7 @@
         <v>30908.863333333331</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" s="95" t="s">
         <v>71</v>
       </c>
@@ -17116,7 +17063,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" s="98" t="s">
         <v>72</v>
       </c>
@@ -17130,7 +17077,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" s="98" t="s">
         <v>72</v>
       </c>
@@ -17144,7 +17091,7 @@
         <v>75702.7</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" s="98" t="s">
         <v>72</v>
       </c>
@@ -17158,7 +17105,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" s="98" t="s">
         <v>72</v>
       </c>
@@ -17172,7 +17119,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" s="98" t="s">
         <v>72</v>
       </c>
@@ -17186,7 +17133,7 @@
         <v>31157.318887999998</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" s="98" t="s">
         <v>72</v>
       </c>
@@ -17200,7 +17147,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" s="98" t="s">
         <v>72</v>
       </c>
@@ -17214,7 +17161,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" s="98" t="s">
         <v>72</v>
       </c>
@@ -17228,7 +17175,7 @@
         <v>5833.333333333333</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" s="95" t="s">
         <v>71</v>
       </c>
@@ -17242,7 +17189,7 @@
         <v>1407.0239328016664</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" s="95" t="s">
         <v>71</v>
       </c>
@@ -17256,7 +17203,7 @@
         <v>11666.666666666666</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" s="95" t="s">
         <v>71</v>
       </c>
@@ -17270,7 +17217,7 @@
         <v>865.16666666666674</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" s="95" t="s">
         <v>71</v>
       </c>
@@ -17284,7 +17231,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" s="95" t="s">
         <v>71</v>
       </c>
@@ -17298,7 +17245,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" s="95" t="s">
         <v>71</v>
       </c>
@@ -17312,7 +17259,7 @@
         <v>19749.776104941466</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" s="95" t="s">
         <v>71</v>
       </c>
@@ -17326,7 +17273,7 @@
         <v>19488.667569444446</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" s="95" t="s">
         <v>71</v>
       </c>
@@ -17340,7 +17287,7 @@
         <v>20833.333333333332</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" s="95" t="s">
         <v>71</v>
       </c>
@@ -17354,7 +17301,7 @@
         <v>1493.13924</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" s="95" t="s">
         <v>71</v>
       </c>
@@ -17368,7 +17315,7 @@
         <v>11277.666666666666</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" s="95" t="s">
         <v>71</v>
       </c>
@@ -17382,7 +17329,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" s="95" t="s">
         <v>71</v>
       </c>
@@ -17396,7 +17343,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" s="95" t="s">
         <v>71</v>
       </c>
@@ -17410,7 +17357,7 @@
         <v>337.06893333333335</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" s="95" t="s">
         <v>71</v>
       </c>
@@ -17424,7 +17371,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" s="95" t="s">
         <v>71</v>
       </c>
@@ -17438,7 +17385,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" s="95" t="s">
         <v>71</v>
       </c>
@@ -17452,7 +17399,7 @@
         <v>833.33333333333337</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" s="95" t="s">
         <v>71</v>
       </c>
@@ -17466,7 +17413,7 @@
         <v>614.26833333333332</v>
       </c>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" s="95" t="s">
         <v>71</v>
       </c>
@@ -17480,7 +17427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" s="95" t="s">
         <v>71</v>
       </c>
@@ -17494,7 +17441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" s="95" t="s">
         <v>71</v>
       </c>
@@ -17508,7 +17455,7 @@
         <v>30908.863333333331</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" s="95" t="s">
         <v>71</v>
       </c>
@@ -17522,7 +17469,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" s="98" t="s">
         <v>72</v>
       </c>
@@ -17536,7 +17483,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" s="98" t="s">
         <v>72</v>
       </c>
@@ -17550,7 +17497,7 @@
         <v>75702.7</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" s="98" t="s">
         <v>72</v>
       </c>
@@ -17564,7 +17511,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" s="98" t="s">
         <v>72</v>
       </c>
@@ -17578,7 +17525,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" s="98" t="s">
         <v>72</v>
       </c>
@@ -17592,7 +17539,7 @@
         <v>31157.318887999998</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" s="98" t="s">
         <v>72</v>
       </c>
@@ -17606,7 +17553,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" s="98" t="s">
         <v>72</v>
       </c>
@@ -17620,7 +17567,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" s="98" t="s">
         <v>72</v>
       </c>
@@ -17634,7 +17581,7 @@
         <v>5833.333333333333</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" s="95" t="s">
         <v>71</v>
       </c>
@@ -17648,7 +17595,7 @@
         <v>1407.0239328016664</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" s="95" t="s">
         <v>71</v>
       </c>
@@ -17662,7 +17609,7 @@
         <v>11666.666666666666</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" s="95" t="s">
         <v>71</v>
       </c>
@@ -17676,7 +17623,7 @@
         <v>865.16666666666674</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" s="95" t="s">
         <v>71</v>
       </c>
@@ -17690,7 +17637,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" s="95" t="s">
         <v>71</v>
       </c>
@@ -17704,7 +17651,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" s="95" t="s">
         <v>71</v>
       </c>
@@ -17718,7 +17665,7 @@
         <v>19749.776104941466</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" s="95" t="s">
         <v>71</v>
       </c>
@@ -17732,7 +17679,7 @@
         <v>19488.667569444446</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" s="95" t="s">
         <v>71</v>
       </c>
@@ -17746,7 +17693,7 @@
         <v>20833.333333333332</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" s="95" t="s">
         <v>71</v>
       </c>
@@ -17760,7 +17707,7 @@
         <v>1493.13924</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" s="95" t="s">
         <v>71</v>
       </c>
@@ -17774,7 +17721,7 @@
         <v>11277.666666666666</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" s="95" t="s">
         <v>71</v>
       </c>
@@ -17788,7 +17735,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" s="95" t="s">
         <v>71</v>
       </c>
@@ -17802,7 +17749,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" s="95" t="s">
         <v>71</v>
       </c>
@@ -17816,7 +17763,7 @@
         <v>337.06893333333335</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" s="95" t="s">
         <v>71</v>
       </c>
@@ -17830,7 +17777,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" s="95" t="s">
         <v>71</v>
       </c>
@@ -17844,7 +17791,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" s="95" t="s">
         <v>71</v>
       </c>
@@ -17858,7 +17805,7 @@
         <v>833.33333333333337</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308" s="95" t="s">
         <v>71</v>
       </c>
@@ -17872,7 +17819,7 @@
         <v>614.26833333333332</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A309" s="95" t="s">
         <v>71</v>
       </c>
@@ -17886,7 +17833,7 @@
         <v>155.72999999999999</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A310" s="95" t="s">
         <v>71</v>
       </c>
@@ -17900,7 +17847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A311" s="95" t="s">
         <v>71</v>
       </c>
@@ -17914,7 +17861,7 @@
         <v>30908.863333333331</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" s="95" t="s">
         <v>71</v>
       </c>
@@ -17928,7 +17875,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" s="98" t="s">
         <v>72</v>
       </c>
@@ -17942,7 +17889,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" s="98" t="s">
         <v>72</v>
       </c>
@@ -17956,7 +17903,7 @@
         <v>75702.7</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315" s="98" t="s">
         <v>72</v>
       </c>
@@ -17970,7 +17917,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" s="98" t="s">
         <v>72</v>
       </c>
@@ -17984,7 +17931,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317" s="98" t="s">
         <v>72</v>
       </c>
@@ -17998,7 +17945,7 @@
         <v>31157.318887999998</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A318" s="98" t="s">
         <v>72</v>
       </c>
@@ -18012,7 +17959,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" s="98" t="s">
         <v>72</v>
       </c>
@@ -18026,7 +17973,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" s="98" t="s">
         <v>72</v>
       </c>
@@ -18040,7 +17987,7 @@
         <v>5833.333333333333</v>
       </c>
     </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A321" s="95" t="s">
         <v>71</v>
       </c>
@@ -18054,7 +18001,7 @@
         <v>1407.0239328016664</v>
       </c>
     </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A322" s="95" t="s">
         <v>71</v>
       </c>
@@ -18068,7 +18015,7 @@
         <v>11666.666666666666</v>
       </c>
     </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A323" s="95" t="s">
         <v>71</v>
       </c>
@@ -18082,7 +18029,7 @@
         <v>865.16666666666674</v>
       </c>
     </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A324" s="95" t="s">
         <v>71</v>
       </c>
@@ -18096,7 +18043,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A325" s="95" t="s">
         <v>71</v>
       </c>
@@ -18110,7 +18057,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A326" s="95" t="s">
         <v>71</v>
       </c>
@@ -18124,7 +18071,7 @@
         <v>19749.776104941466</v>
       </c>
     </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A327" s="95" t="s">
         <v>71</v>
       </c>
@@ -18138,7 +18085,7 @@
         <v>19488.667569444446</v>
       </c>
     </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A328" s="95" t="s">
         <v>71</v>
       </c>
@@ -18152,7 +18099,7 @@
         <v>20833.333333333332</v>
       </c>
     </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A329" s="95" t="s">
         <v>71</v>
       </c>
@@ -18166,7 +18113,7 @@
         <v>1493.13924</v>
       </c>
     </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A330" s="95" t="s">
         <v>71</v>
       </c>
@@ -18180,7 +18127,7 @@
         <v>11277.666666666666</v>
       </c>
     </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A331" s="95" t="s">
         <v>71</v>
       </c>
@@ -18194,7 +18141,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="332" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A332" s="95" t="s">
         <v>71</v>
       </c>
@@ -18208,7 +18155,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="333" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A333" s="95" t="s">
         <v>71</v>
       </c>
@@ -18222,7 +18169,7 @@
         <v>337.06893333333335</v>
       </c>
     </row>
-    <row r="334" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A334" s="95" t="s">
         <v>71</v>
       </c>
@@ -18236,7 +18183,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="335" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A335" s="95" t="s">
         <v>71</v>
       </c>
@@ -18250,7 +18197,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="336" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A336" s="95" t="s">
         <v>71</v>
       </c>
@@ -18264,7 +18211,7 @@
         <v>833.33333333333337</v>
       </c>
     </row>
-    <row r="337" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A337" s="95" t="s">
         <v>71</v>
       </c>
@@ -18278,7 +18225,7 @@
         <v>614.26833333333332</v>
       </c>
     </row>
-    <row r="338" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A338" s="95" t="s">
         <v>71</v>
       </c>
@@ -18292,7 +18239,7 @@
         <v>1483.5878</v>
       </c>
     </row>
-    <row r="339" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A339" s="95" t="s">
         <v>71</v>
       </c>
@@ -18306,7 +18253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A340" s="95" t="s">
         <v>71</v>
       </c>
@@ -18320,7 +18267,7 @@
         <v>30908.863333333331</v>
       </c>
     </row>
-    <row r="341" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A341" s="95" t="s">
         <v>71</v>
       </c>
@@ -18334,7 +18281,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="342" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A342" s="98" t="s">
         <v>72</v>
       </c>
@@ -18348,7 +18295,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="343" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" s="98" t="s">
         <v>72</v>
       </c>
@@ -18362,7 +18309,7 @@
         <v>75702.7</v>
       </c>
     </row>
-    <row r="344" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A344" s="98" t="s">
         <v>72</v>
       </c>
@@ -18376,7 +18323,7 @@
         <v>1730.3333333333335</v>
       </c>
     </row>
-    <row r="345" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A345" s="98" t="s">
         <v>72</v>
       </c>
@@ -18390,7 +18337,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="346" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A346" s="98" t="s">
         <v>72</v>
       </c>
@@ -18404,7 +18351,7 @@
         <v>31157.318887999998</v>
       </c>
     </row>
-    <row r="347" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A347" s="98" t="s">
         <v>72</v>
       </c>
@@ -18418,7 +18365,7 @@
         <v>8333.3333333333339</v>
       </c>
     </row>
-    <row r="348" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A348" s="98" t="s">
         <v>72</v>
       </c>
@@ -18432,7 +18379,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="349" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A349" s="98" t="s">
         <v>72</v>
       </c>

</xml_diff>